<commit_message>
Add displacement and reaction calculation to structure analysis
Todo bien menos las reacciones, se corrigieron muchas cosas, zzz
Enhanced the structural analysis workflow by implementing methods to solve for nodal displacements and calculate support reactions in Estructura. Updated the test script to use these features and export results to Excel. Fixed the local stiffness matrix assembly in Barra for correct 3D frame behavior. Adjusted test data for loads and boundary conditions.
</commit_message>
<xml_diff>
--- a/matrices_rigidez_3D.xlsx
+++ b/matrices_rigidez_3D.xlsx
@@ -10,6 +10,9 @@
     <sheet name="Barra 1 (K1)" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Barra 2 (K2)" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Global" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="F" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Desplazamientos" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Reacciones" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,10 +428,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>2016</v>
+        <v>4032</v>
       </c>
       <c r="B1" t="n">
-        <v>-5040</v>
+        <v>0</v>
       </c>
       <c r="C1" t="n">
         <v>0</v>
@@ -437,13 +440,13 @@
         <v>0</v>
       </c>
       <c r="E1" t="n">
-        <v>-5040</v>
+        <v>10080</v>
       </c>
       <c r="F1" t="n">
-        <v>5040</v>
+        <v>0</v>
       </c>
       <c r="G1" t="n">
-        <v>0</v>
+        <v>-4032</v>
       </c>
       <c r="H1" t="n">
         <v>0</v>
@@ -455,7 +458,7 @@
         <v>0</v>
       </c>
       <c r="K1" t="n">
-        <v>0</v>
+        <v>10080</v>
       </c>
       <c r="L1" t="n">
         <v>0</v>
@@ -463,7 +466,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-5040</v>
+        <v>0</v>
       </c>
       <c r="B2" t="n">
         <v>2016</v>
@@ -472,25 +475,25 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>5040</v>
+        <v>-5040</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
       </c>
       <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
         <v>-2016</v>
       </c>
-      <c r="G2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0</v>
-      </c>
       <c r="I2" t="n">
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>-5040</v>
       </c>
       <c r="K2" t="n">
         <v>0</v>
@@ -525,7 +528,7 @@
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>-42000</v>
       </c>
       <c r="J3" t="n">
         <v>0</v>
@@ -542,7 +545,7 @@
         <v>0</v>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>-5040</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
@@ -551,7 +554,7 @@
         <v>16800</v>
       </c>
       <c r="E4" t="n">
-        <v>-5040</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
@@ -560,13 +563,13 @@
         <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>5040</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>0</v>
+        <v>8400</v>
       </c>
       <c r="K4" t="n">
         <v>0</v>
@@ -577,7 +580,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0</v>
+        <v>10080</v>
       </c>
       <c r="B5" t="n">
         <v>0</v>
@@ -586,28 +589,28 @@
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>-5040</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
+        <v>33600</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>-10080</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
         <v>16800</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" t="n">
-        <v>0</v>
       </c>
       <c r="L5" t="n">
         <v>0</v>
@@ -615,10 +618,10 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>5040</v>
+        <v>0</v>
       </c>
       <c r="B6" t="n">
-        <v>-2016</v>
+        <v>0</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
@@ -648,12 +651,12 @@
         <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>0</v>
+        <v>-800</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0</v>
+        <v>-4032</v>
       </c>
       <c r="B7" t="n">
         <v>0</v>
@@ -665,13 +668,13 @@
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>-10080</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>2016</v>
+        <v>4032</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -683,7 +686,7 @@
         <v>0</v>
       </c>
       <c r="K7" t="n">
-        <v>0</v>
+        <v>-10080</v>
       </c>
       <c r="L7" t="n">
         <v>0</v>
@@ -694,13 +697,13 @@
         <v>0</v>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>-2016</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>5040</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
@@ -718,7 +721,7 @@
         <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>0</v>
+        <v>5040</v>
       </c>
       <c r="K8" t="n">
         <v>0</v>
@@ -735,7 +738,7 @@
         <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>-42000</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
@@ -770,13 +773,13 @@
         <v>0</v>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>-5040</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>8400</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
@@ -788,7 +791,7 @@
         <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>5040</v>
       </c>
       <c r="I10" t="n">
         <v>0</v>
@@ -805,7 +808,7 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0</v>
+        <v>10080</v>
       </c>
       <c r="B11" t="n">
         <v>0</v>
@@ -817,13 +820,13 @@
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>16800</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>-10080</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
@@ -835,7 +838,7 @@
         <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>16800</v>
+        <v>33600</v>
       </c>
       <c r="L11" t="n">
         <v>0</v>
@@ -858,7 +861,7 @@
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>-800</v>
       </c>
       <c r="G12" t="n">
         <v>0</v>
@@ -900,10 +903,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>2016</v>
+        <v>4032</v>
       </c>
       <c r="B1" t="n">
-        <v>-5040</v>
+        <v>0</v>
       </c>
       <c r="C1" t="n">
         <v>0</v>
@@ -912,13 +915,13 @@
         <v>0</v>
       </c>
       <c r="E1" t="n">
-        <v>-5040</v>
+        <v>10080</v>
       </c>
       <c r="F1" t="n">
-        <v>5040</v>
+        <v>0</v>
       </c>
       <c r="G1" t="n">
-        <v>0</v>
+        <v>-4032</v>
       </c>
       <c r="H1" t="n">
         <v>0</v>
@@ -930,7 +933,7 @@
         <v>0</v>
       </c>
       <c r="K1" t="n">
-        <v>0</v>
+        <v>10080</v>
       </c>
       <c r="L1" t="n">
         <v>0</v>
@@ -938,7 +941,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-5040</v>
+        <v>0</v>
       </c>
       <c r="B2" t="n">
         <v>2016</v>
@@ -947,25 +950,25 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>5040</v>
+        <v>-5040</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
       </c>
       <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
         <v>-2016</v>
       </c>
-      <c r="G2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0</v>
-      </c>
       <c r="I2" t="n">
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>-5040</v>
       </c>
       <c r="K2" t="n">
         <v>0</v>
@@ -1000,7 +1003,7 @@
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>-42000</v>
       </c>
       <c r="J3" t="n">
         <v>0</v>
@@ -1017,7 +1020,7 @@
         <v>0</v>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>-5040</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
@@ -1026,7 +1029,7 @@
         <v>16800</v>
       </c>
       <c r="E4" t="n">
-        <v>-5040</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
@@ -1035,13 +1038,13 @@
         <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>5040</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>0</v>
+        <v>8400</v>
       </c>
       <c r="K4" t="n">
         <v>0</v>
@@ -1052,7 +1055,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0</v>
+        <v>10080</v>
       </c>
       <c r="B5" t="n">
         <v>0</v>
@@ -1061,28 +1064,28 @@
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>-5040</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
+        <v>33600</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>-10080</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
         <v>16800</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" t="n">
-        <v>0</v>
       </c>
       <c r="L5" t="n">
         <v>0</v>
@@ -1090,10 +1093,10 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>5040</v>
+        <v>0</v>
       </c>
       <c r="B6" t="n">
-        <v>-2016</v>
+        <v>0</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
@@ -1123,12 +1126,12 @@
         <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>0</v>
+        <v>-800</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0</v>
+        <v>-4032</v>
       </c>
       <c r="B7" t="n">
         <v>0</v>
@@ -1140,13 +1143,13 @@
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>-10080</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>2016</v>
+        <v>4032</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -1158,7 +1161,7 @@
         <v>0</v>
       </c>
       <c r="K7" t="n">
-        <v>0</v>
+        <v>-10080</v>
       </c>
       <c r="L7" t="n">
         <v>0</v>
@@ -1169,13 +1172,13 @@
         <v>0</v>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>-2016</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>5040</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
@@ -1193,7 +1196,7 @@
         <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>0</v>
+        <v>5040</v>
       </c>
       <c r="K8" t="n">
         <v>0</v>
@@ -1210,7 +1213,7 @@
         <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>-42000</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
@@ -1245,13 +1248,13 @@
         <v>0</v>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>-5040</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>8400</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
@@ -1263,7 +1266,7 @@
         <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>5040</v>
       </c>
       <c r="I10" t="n">
         <v>0</v>
@@ -1280,7 +1283,7 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0</v>
+        <v>10080</v>
       </c>
       <c r="B11" t="n">
         <v>0</v>
@@ -1292,13 +1295,13 @@
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>16800</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>-10080</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
@@ -1310,7 +1313,7 @@
         <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>16800</v>
+        <v>33600</v>
       </c>
       <c r="L11" t="n">
         <v>0</v>
@@ -1333,7 +1336,7 @@
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>-800</v>
       </c>
       <c r="G12" t="n">
         <v>0</v>
@@ -1375,10 +1378,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>2016</v>
+        <v>4032</v>
       </c>
       <c r="B1" t="n">
-        <v>-5040</v>
+        <v>0</v>
       </c>
       <c r="C1" t="n">
         <v>0</v>
@@ -1387,13 +1390,13 @@
         <v>0</v>
       </c>
       <c r="E1" t="n">
-        <v>-5040</v>
+        <v>10080</v>
       </c>
       <c r="F1" t="n">
-        <v>5040</v>
+        <v>0</v>
       </c>
       <c r="G1" t="n">
-        <v>0</v>
+        <v>-4032</v>
       </c>
       <c r="H1" t="n">
         <v>0</v>
@@ -1405,7 +1408,7 @@
         <v>0</v>
       </c>
       <c r="K1" t="n">
-        <v>0</v>
+        <v>10080</v>
       </c>
       <c r="L1" t="n">
         <v>0</v>
@@ -1431,7 +1434,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-5040</v>
+        <v>0</v>
       </c>
       <c r="B2" t="n">
         <v>2016</v>
@@ -1440,25 +1443,25 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>5040</v>
+        <v>-5040</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
       </c>
       <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
         <v>-2016</v>
       </c>
-      <c r="G2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0</v>
-      </c>
       <c r="I2" t="n">
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>-5040</v>
       </c>
       <c r="K2" t="n">
         <v>0</v>
@@ -1511,7 +1514,7 @@
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>-42000</v>
       </c>
       <c r="J3" t="n">
         <v>0</v>
@@ -1546,7 +1549,7 @@
         <v>0</v>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>-5040</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
@@ -1555,7 +1558,7 @@
         <v>16800</v>
       </c>
       <c r="E4" t="n">
-        <v>-5040</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
@@ -1564,13 +1567,13 @@
         <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>5040</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>0</v>
+        <v>8400</v>
       </c>
       <c r="K4" t="n">
         <v>0</v>
@@ -1599,7 +1602,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0</v>
+        <v>10080</v>
       </c>
       <c r="B5" t="n">
         <v>0</v>
@@ -1608,28 +1611,28 @@
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>-5040</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
+        <v>33600</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>-10080</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
         <v>16800</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" t="n">
-        <v>0</v>
       </c>
       <c r="L5" t="n">
         <v>0</v>
@@ -1655,10 +1658,10 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>5040</v>
+        <v>0</v>
       </c>
       <c r="B6" t="n">
-        <v>-2016</v>
+        <v>0</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
@@ -1688,7 +1691,7 @@
         <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>0</v>
+        <v>-800</v>
       </c>
       <c r="M6" t="n">
         <v>0</v>
@@ -1711,7 +1714,7 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0</v>
+        <v>-4032</v>
       </c>
       <c r="B7" t="n">
         <v>0</v>
@@ -1723,16 +1726,16 @@
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>-10080</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>4032</v>
+        <v>8064</v>
       </c>
       <c r="H7" t="n">
-        <v>-5040</v>
+        <v>0</v>
       </c>
       <c r="I7" t="n">
         <v>0</v>
@@ -1741,13 +1744,13 @@
         <v>0</v>
       </c>
       <c r="K7" t="n">
-        <v>-5040</v>
+        <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>5040</v>
+        <v>0</v>
       </c>
       <c r="M7" t="n">
-        <v>0</v>
+        <v>-4032</v>
       </c>
       <c r="N7" t="n">
         <v>0</v>
@@ -1759,7 +1762,7 @@
         <v>0</v>
       </c>
       <c r="Q7" t="n">
-        <v>0</v>
+        <v>10080</v>
       </c>
       <c r="R7" t="n">
         <v>0</v>
@@ -1770,13 +1773,13 @@
         <v>0</v>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>-2016</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>5040</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
@@ -1785,7 +1788,7 @@
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>-5040</v>
+        <v>0</v>
       </c>
       <c r="H8" t="n">
         <v>4032</v>
@@ -1794,25 +1797,25 @@
         <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>5040</v>
+        <v>0</v>
       </c>
       <c r="K8" t="n">
         <v>0</v>
       </c>
       <c r="L8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" t="n">
         <v>-2016</v>
       </c>
-      <c r="M8" t="n">
-        <v>0</v>
-      </c>
-      <c r="N8" t="n">
-        <v>0</v>
-      </c>
       <c r="O8" t="n">
         <v>0</v>
       </c>
       <c r="P8" t="n">
-        <v>0</v>
+        <v>-5040</v>
       </c>
       <c r="Q8" t="n">
         <v>0</v>
@@ -1829,7 +1832,7 @@
         <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>-42000</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
@@ -1865,7 +1868,7 @@
         <v>0</v>
       </c>
       <c r="O9" t="n">
-        <v>0</v>
+        <v>-42000</v>
       </c>
       <c r="P9" t="n">
         <v>0</v>
@@ -1882,13 +1885,13 @@
         <v>0</v>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>-5040</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>8400</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
@@ -1909,7 +1912,7 @@
         <v>33600</v>
       </c>
       <c r="K10" t="n">
-        <v>-5040</v>
+        <v>0</v>
       </c>
       <c r="L10" t="n">
         <v>0</v>
@@ -1918,13 +1921,13 @@
         <v>0</v>
       </c>
       <c r="N10" t="n">
-        <v>0</v>
+        <v>5040</v>
       </c>
       <c r="O10" t="n">
         <v>0</v>
       </c>
       <c r="P10" t="n">
-        <v>0</v>
+        <v>8400</v>
       </c>
       <c r="Q10" t="n">
         <v>0</v>
@@ -1935,7 +1938,7 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0</v>
+        <v>10080</v>
       </c>
       <c r="B11" t="n">
         <v>0</v>
@@ -1947,7 +1950,7 @@
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>16800</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
@@ -1962,16 +1965,16 @@
         <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>-5040</v>
+        <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>33600</v>
+        <v>67200</v>
       </c>
       <c r="L11" t="n">
         <v>0</v>
       </c>
       <c r="M11" t="n">
-        <v>0</v>
+        <v>-10080</v>
       </c>
       <c r="N11" t="n">
         <v>0</v>
@@ -1983,7 +1986,7 @@
         <v>0</v>
       </c>
       <c r="Q11" t="n">
-        <v>0</v>
+        <v>16800</v>
       </c>
       <c r="R11" t="n">
         <v>0</v>
@@ -2006,13 +2009,13 @@
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>-800</v>
       </c>
       <c r="G12" t="n">
-        <v>5040</v>
+        <v>0</v>
       </c>
       <c r="H12" t="n">
-        <v>-2016</v>
+        <v>0</v>
       </c>
       <c r="I12" t="n">
         <v>0</v>
@@ -2042,7 +2045,7 @@
         <v>0</v>
       </c>
       <c r="R12" t="n">
-        <v>0</v>
+        <v>-800</v>
       </c>
     </row>
     <row r="13">
@@ -2065,7 +2068,7 @@
         <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>-4032</v>
       </c>
       <c r="H13" t="n">
         <v>0</v>
@@ -2077,13 +2080,13 @@
         <v>0</v>
       </c>
       <c r="K13" t="n">
-        <v>0</v>
+        <v>-10080</v>
       </c>
       <c r="L13" t="n">
         <v>0</v>
       </c>
       <c r="M13" t="n">
-        <v>2016</v>
+        <v>4032</v>
       </c>
       <c r="N13" t="n">
         <v>0</v>
@@ -2095,7 +2098,7 @@
         <v>0</v>
       </c>
       <c r="Q13" t="n">
-        <v>0</v>
+        <v>-10080</v>
       </c>
       <c r="R13" t="n">
         <v>0</v>
@@ -2124,13 +2127,13 @@
         <v>0</v>
       </c>
       <c r="H14" t="n">
-        <v>0</v>
+        <v>-2016</v>
       </c>
       <c r="I14" t="n">
         <v>0</v>
       </c>
       <c r="J14" t="n">
-        <v>0</v>
+        <v>5040</v>
       </c>
       <c r="K14" t="n">
         <v>0</v>
@@ -2148,7 +2151,7 @@
         <v>0</v>
       </c>
       <c r="P14" t="n">
-        <v>0</v>
+        <v>5040</v>
       </c>
       <c r="Q14" t="n">
         <v>0</v>
@@ -2183,7 +2186,7 @@
         <v>0</v>
       </c>
       <c r="I15" t="n">
-        <v>0</v>
+        <v>-42000</v>
       </c>
       <c r="J15" t="n">
         <v>0</v>
@@ -2236,13 +2239,13 @@
         <v>0</v>
       </c>
       <c r="H16" t="n">
-        <v>0</v>
+        <v>-5040</v>
       </c>
       <c r="I16" t="n">
         <v>0</v>
       </c>
       <c r="J16" t="n">
-        <v>0</v>
+        <v>8400</v>
       </c>
       <c r="K16" t="n">
         <v>0</v>
@@ -2254,7 +2257,7 @@
         <v>0</v>
       </c>
       <c r="N16" t="n">
-        <v>0</v>
+        <v>5040</v>
       </c>
       <c r="O16" t="n">
         <v>0</v>
@@ -2289,7 +2292,7 @@
         <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>0</v>
+        <v>10080</v>
       </c>
       <c r="H17" t="n">
         <v>0</v>
@@ -2301,13 +2304,13 @@
         <v>0</v>
       </c>
       <c r="K17" t="n">
-        <v>0</v>
+        <v>16800</v>
       </c>
       <c r="L17" t="n">
         <v>0</v>
       </c>
       <c r="M17" t="n">
-        <v>0</v>
+        <v>-10080</v>
       </c>
       <c r="N17" t="n">
         <v>0</v>
@@ -2319,7 +2322,7 @@
         <v>0</v>
       </c>
       <c r="Q17" t="n">
-        <v>16800</v>
+        <v>33600</v>
       </c>
       <c r="R17" t="n">
         <v>0</v>
@@ -2360,7 +2363,7 @@
         <v>0</v>
       </c>
       <c r="L18" t="n">
-        <v>0</v>
+        <v>-800</v>
       </c>
       <c r="M18" t="n">
         <v>0</v>
@@ -2379,6 +2382,333 @@
       </c>
       <c r="R18" t="n">
         <v>800</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="n">
+        <v>-3.673940397442059e-14</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>-648</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>-3.967855629237424e-14</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>-4.408728476930472e-14</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>-720</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>-6.123233995736766e-14</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>-6.123233995736768e-14</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>-1.469576158976824e-14</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>-239.9999999999999</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>-2.449293598294707e-14</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>-352.0000000000001</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>-2.155378366499342e-14</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>2.939152317953648e-14</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>480.0000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>-7.593296125665633e-18</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>-0.2480158730158731</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>-7.289564280639009e-19</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>-2.186869284191702e-19</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>-0.1499999999999999</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="n">
+        <v>6.515120971463919e-14</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>7.029472627105808e-14</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>-1250</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1.169537693185722e-13</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>5.731347020009613e-14</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>852.0000000000002</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>5.216995364367726e-14</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>-1.096058885236881e-13</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>-360.0000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ESTO ES PARA GUARDAR UNA COPIA
guardar una copia antes de hacer un supercambio xd
</commit_message>
<xml_diff>
--- a/matrices_rigidez_3D.xlsx
+++ b/matrices_rigidez_3D.xlsx
@@ -1383,42 +1383,42 @@
         <v>2136.96</v>
       </c>
       <c r="B1" t="n">
-        <v>-1.069028481086101e-13</v>
+        <v>1.069028481086101e-13</v>
       </c>
       <c r="C1" t="n">
-        <v>-1.282793029170869e-13</v>
+        <v>1.282793029170869e-13</v>
       </c>
       <c r="D1" t="n">
         <v>2.672571202715251e-13</v>
       </c>
       <c r="E1" t="n">
-        <v>5342.4</v>
+        <v>-5342.4</v>
       </c>
       <c r="F1" t="n">
-        <v>-1.636477884449312e-29</v>
+        <v>1.636477884449312e-29</v>
       </c>
       <c r="G1" t="n">
         <v>-2136.96</v>
       </c>
       <c r="H1" t="n">
-        <v>1.069028481086101e-13</v>
+        <v>-1.069028481086101e-13</v>
       </c>
       <c r="I1" t="n">
-        <v>1.282793029170869e-13</v>
+        <v>-1.282793029170869e-13</v>
       </c>
       <c r="J1" t="n">
         <v>2.672571202715251e-13</v>
       </c>
       <c r="K1" t="n">
-        <v>5342.4</v>
+        <v>-5342.4</v>
       </c>
       <c r="L1" t="n">
-        <v>-1.636477884449312e-29</v>
+        <v>1.636477884449312e-29</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-1.069028481086101e-13</v>
+        <v>1.069028481086101e-13</v>
       </c>
       <c r="B2" t="n">
         <v>391.104</v>
@@ -1427,7 +1427,7 @@
         <v>6.545911537797249e-30</v>
       </c>
       <c r="D2" t="n">
-        <v>-977.76</v>
+        <v>977.76</v>
       </c>
       <c r="E2" t="n">
         <v>-2.672571202715251e-13</v>
@@ -1436,7 +1436,7 @@
         <v>5.987053271671581e-14</v>
       </c>
       <c r="G2" t="n">
-        <v>1.069028481086101e-13</v>
+        <v>-1.069028481086101e-13</v>
       </c>
       <c r="H2" t="n">
         <v>-391.104</v>
@@ -1445,7 +1445,7 @@
         <v>-6.545911537797249e-30</v>
       </c>
       <c r="J2" t="n">
-        <v>-977.76</v>
+        <v>977.76</v>
       </c>
       <c r="K2" t="n">
         <v>-2.672571202715251e-13</v>
@@ -1456,7 +1456,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>-1.282793029170869e-13</v>
+        <v>1.282793029170869e-13</v>
       </c>
       <c r="B3" t="n">
         <v>6.545911537797249e-30</v>
@@ -1465,7 +1465,7 @@
         <v>42</v>
       </c>
       <c r="D3" t="n">
-        <v>-1.636477884449312e-29</v>
+        <v>1.636477884449312e-29</v>
       </c>
       <c r="E3" t="n">
         <v>-3.27127652988241e-13</v>
@@ -1474,7 +1474,7 @@
         <v>1.002053701533141e-45</v>
       </c>
       <c r="G3" t="n">
-        <v>1.282793029170869e-13</v>
+        <v>-1.282793029170869e-13</v>
       </c>
       <c r="H3" t="n">
         <v>-6.545911537797249e-30</v>
@@ -1483,7 +1483,7 @@
         <v>-42</v>
       </c>
       <c r="J3" t="n">
-        <v>-1.636477884449312e-29</v>
+        <v>1.636477884449312e-29</v>
       </c>
       <c r="K3" t="n">
         <v>-3.27127652988241e-13</v>
@@ -1497,42 +1497,42 @@
         <v>2.672571202715251e-13</v>
       </c>
       <c r="B4" t="n">
-        <v>-977.76</v>
+        <v>977.76</v>
       </c>
       <c r="C4" t="n">
-        <v>-1.636477884449312e-29</v>
+        <v>1.636477884449312e-29</v>
       </c>
       <c r="D4" t="n">
         <v>3259.2</v>
       </c>
       <c r="E4" t="n">
-        <v>8.908570675717507e-13</v>
+        <v>-8.908570675717507e-13</v>
       </c>
       <c r="F4" t="n">
-        <v>-1.9759014794971e-13</v>
+        <v>1.9759014794971e-13</v>
       </c>
       <c r="G4" t="n">
         <v>-2.672571202715251e-13</v>
       </c>
       <c r="H4" t="n">
-        <v>977.76</v>
+        <v>-977.76</v>
       </c>
       <c r="I4" t="n">
-        <v>1.636477884449312e-29</v>
+        <v>-1.636477884449312e-29</v>
       </c>
       <c r="J4" t="n">
         <v>1629.6</v>
       </c>
       <c r="K4" t="n">
-        <v>4.454285337858754e-13</v>
+        <v>-4.454285337858754e-13</v>
       </c>
       <c r="L4" t="n">
-        <v>-1.01762515633869e-13</v>
+        <v>1.01762515633869e-13</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>5342.4</v>
+        <v>-5342.4</v>
       </c>
       <c r="B5" t="n">
         <v>-2.672571202715251e-13</v>
@@ -1541,7 +1541,7 @@
         <v>-3.27127652988241e-13</v>
       </c>
       <c r="D5" t="n">
-        <v>8.908570675717506e-13</v>
+        <v>-8.908570675717506e-13</v>
       </c>
       <c r="E5" t="n">
         <v>17808</v>
@@ -1550,7 +1550,7 @@
         <v>-5.454926281497708e-29</v>
       </c>
       <c r="G5" t="n">
-        <v>-5342.4</v>
+        <v>5342.4</v>
       </c>
       <c r="H5" t="n">
         <v>2.672571202715251e-13</v>
@@ -1559,7 +1559,7 @@
         <v>3.27127652988241e-13</v>
       </c>
       <c r="J5" t="n">
-        <v>4.454285337858753e-13</v>
+        <v>-4.454285337858753e-13</v>
       </c>
       <c r="K5" t="n">
         <v>8904</v>
@@ -1570,7 +1570,7 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-1.636477884449312e-29</v>
+        <v>1.636477884449312e-29</v>
       </c>
       <c r="B6" t="n">
         <v>5.987053271671581e-14</v>
@@ -1579,7 +1579,7 @@
         <v>1.002053701533141e-45</v>
       </c>
       <c r="D6" t="n">
-        <v>-1.9759014794971e-13</v>
+        <v>1.9759014794971e-13</v>
       </c>
       <c r="E6" t="n">
         <v>-5.454926281497709e-29</v>
@@ -1588,7 +1588,7 @@
         <v>32.308</v>
       </c>
       <c r="G6" t="n">
-        <v>1.636477884449312e-29</v>
+        <v>-1.636477884449312e-29</v>
       </c>
       <c r="H6" t="n">
         <v>-5.987053271671581e-14</v>
@@ -1597,7 +1597,7 @@
         <v>-1.002053701533141e-45</v>
       </c>
       <c r="J6" t="n">
-        <v>-1.01762515633869e-13</v>
+        <v>1.01762515633869e-13</v>
       </c>
       <c r="K6" t="n">
         <v>-2.727463140748855e-29</v>
@@ -1611,42 +1611,42 @@
         <v>-2136.96</v>
       </c>
       <c r="B7" t="n">
-        <v>1.069028481086101e-13</v>
+        <v>-1.069028481086101e-13</v>
       </c>
       <c r="C7" t="n">
-        <v>1.282793029170869e-13</v>
+        <v>-1.282793029170869e-13</v>
       </c>
       <c r="D7" t="n">
         <v>-2.672571202715251e-13</v>
       </c>
       <c r="E7" t="n">
-        <v>-5342.4</v>
+        <v>5342.4</v>
       </c>
       <c r="F7" t="n">
-        <v>1.636477884449312e-29</v>
+        <v>-1.636477884449312e-29</v>
       </c>
       <c r="G7" t="n">
         <v>2136.96</v>
       </c>
       <c r="H7" t="n">
-        <v>-1.069028481086101e-13</v>
+        <v>1.069028481086101e-13</v>
       </c>
       <c r="I7" t="n">
-        <v>-1.282793029170869e-13</v>
+        <v>1.282793029170869e-13</v>
       </c>
       <c r="J7" t="n">
         <v>-2.672571202715251e-13</v>
       </c>
       <c r="K7" t="n">
-        <v>-5342.4</v>
+        <v>5342.4</v>
       </c>
       <c r="L7" t="n">
-        <v>1.636477884449312e-29</v>
+        <v>-1.636477884449312e-29</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1.069028481086101e-13</v>
+        <v>-1.069028481086101e-13</v>
       </c>
       <c r="B8" t="n">
         <v>-391.104</v>
@@ -1655,7 +1655,7 @@
         <v>-6.545911537797249e-30</v>
       </c>
       <c r="D8" t="n">
-        <v>977.76</v>
+        <v>-977.76</v>
       </c>
       <c r="E8" t="n">
         <v>2.672571202715251e-13</v>
@@ -1664,7 +1664,7 @@
         <v>-5.987053271671581e-14</v>
       </c>
       <c r="G8" t="n">
-        <v>-1.069028481086101e-13</v>
+        <v>1.069028481086101e-13</v>
       </c>
       <c r="H8" t="n">
         <v>391.104</v>
@@ -1673,7 +1673,7 @@
         <v>6.545911537797249e-30</v>
       </c>
       <c r="J8" t="n">
-        <v>977.76</v>
+        <v>-977.76</v>
       </c>
       <c r="K8" t="n">
         <v>2.672571202715251e-13</v>
@@ -1684,7 +1684,7 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1.282793029170869e-13</v>
+        <v>-1.282793029170869e-13</v>
       </c>
       <c r="B9" t="n">
         <v>-6.545911537797249e-30</v>
@@ -1693,7 +1693,7 @@
         <v>-42</v>
       </c>
       <c r="D9" t="n">
-        <v>1.636477884449312e-29</v>
+        <v>-1.636477884449312e-29</v>
       </c>
       <c r="E9" t="n">
         <v>3.27127652988241e-13</v>
@@ -1702,7 +1702,7 @@
         <v>-1.002053701533141e-45</v>
       </c>
       <c r="G9" t="n">
-        <v>-1.282793029170869e-13</v>
+        <v>1.282793029170869e-13</v>
       </c>
       <c r="H9" t="n">
         <v>6.545911537797249e-30</v>
@@ -1711,7 +1711,7 @@
         <v>42</v>
       </c>
       <c r="J9" t="n">
-        <v>1.636477884449312e-29</v>
+        <v>-1.636477884449312e-29</v>
       </c>
       <c r="K9" t="n">
         <v>3.27127652988241e-13</v>
@@ -1725,42 +1725,42 @@
         <v>2.672571202715251e-13</v>
       </c>
       <c r="B10" t="n">
-        <v>-977.76</v>
+        <v>977.76</v>
       </c>
       <c r="C10" t="n">
-        <v>-1.636477884449312e-29</v>
+        <v>1.636477884449312e-29</v>
       </c>
       <c r="D10" t="n">
         <v>1629.6</v>
       </c>
       <c r="E10" t="n">
-        <v>4.454285337858754e-13</v>
+        <v>-4.454285337858754e-13</v>
       </c>
       <c r="F10" t="n">
-        <v>-1.01762515633869e-13</v>
+        <v>1.01762515633869e-13</v>
       </c>
       <c r="G10" t="n">
         <v>-2.672571202715251e-13</v>
       </c>
       <c r="H10" t="n">
-        <v>977.76</v>
+        <v>-977.76</v>
       </c>
       <c r="I10" t="n">
-        <v>1.636477884449312e-29</v>
+        <v>-1.636477884449312e-29</v>
       </c>
       <c r="J10" t="n">
         <v>3259.2</v>
       </c>
       <c r="K10" t="n">
-        <v>8.908570675717507e-13</v>
+        <v>-8.908570675717507e-13</v>
       </c>
       <c r="L10" t="n">
-        <v>-1.9759014794971e-13</v>
+        <v>1.9759014794971e-13</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>5342.4</v>
+        <v>-5342.4</v>
       </c>
       <c r="B11" t="n">
         <v>-2.672571202715251e-13</v>
@@ -1769,7 +1769,7 @@
         <v>-3.27127652988241e-13</v>
       </c>
       <c r="D11" t="n">
-        <v>4.454285337858753e-13</v>
+        <v>-4.454285337858753e-13</v>
       </c>
       <c r="E11" t="n">
         <v>8904</v>
@@ -1778,7 +1778,7 @@
         <v>-2.727463140748854e-29</v>
       </c>
       <c r="G11" t="n">
-        <v>-5342.4</v>
+        <v>5342.4</v>
       </c>
       <c r="H11" t="n">
         <v>2.672571202715251e-13</v>
@@ -1787,7 +1787,7 @@
         <v>3.27127652988241e-13</v>
       </c>
       <c r="J11" t="n">
-        <v>8.908570675717506e-13</v>
+        <v>-8.908570675717506e-13</v>
       </c>
       <c r="K11" t="n">
         <v>17808</v>
@@ -1798,7 +1798,7 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>-1.636477884449312e-29</v>
+        <v>1.636477884449312e-29</v>
       </c>
       <c r="B12" t="n">
         <v>5.987053271671581e-14</v>
@@ -1807,7 +1807,7 @@
         <v>1.002053701533141e-45</v>
       </c>
       <c r="D12" t="n">
-        <v>-1.01762515633869e-13</v>
+        <v>1.01762515633869e-13</v>
       </c>
       <c r="E12" t="n">
         <v>-2.727463140748855e-29</v>
@@ -1816,7 +1816,7 @@
         <v>-32.308</v>
       </c>
       <c r="G12" t="n">
-        <v>1.636477884449312e-29</v>
+        <v>-1.636477884449312e-29</v>
       </c>
       <c r="H12" t="n">
         <v>-5.987053271671581e-14</v>
@@ -1825,7 +1825,7 @@
         <v>-1.002053701533141e-45</v>
       </c>
       <c r="J12" t="n">
-        <v>-1.9759014794971e-13</v>
+        <v>1.9759014794971e-13</v>
       </c>
       <c r="K12" t="n">
         <v>-5.454926281497709e-29</v>
@@ -1858,42 +1858,42 @@
         <v>2136.96</v>
       </c>
       <c r="B1" t="n">
-        <v>-1.069028481086101e-13</v>
+        <v>1.069028481086101e-13</v>
       </c>
       <c r="C1" t="n">
-        <v>-1.282793029170869e-13</v>
+        <v>1.282793029170869e-13</v>
       </c>
       <c r="D1" t="n">
         <v>2.672571202715251e-13</v>
       </c>
       <c r="E1" t="n">
-        <v>5342.4</v>
+        <v>-5342.4</v>
       </c>
       <c r="F1" t="n">
-        <v>-1.636477884449312e-29</v>
+        <v>1.636477884449312e-29</v>
       </c>
       <c r="G1" t="n">
         <v>-2136.96</v>
       </c>
       <c r="H1" t="n">
-        <v>1.069028481086101e-13</v>
+        <v>-1.069028481086101e-13</v>
       </c>
       <c r="I1" t="n">
-        <v>1.282793029170869e-13</v>
+        <v>-1.282793029170869e-13</v>
       </c>
       <c r="J1" t="n">
         <v>2.672571202715251e-13</v>
       </c>
       <c r="K1" t="n">
-        <v>5342.4</v>
+        <v>-5342.4</v>
       </c>
       <c r="L1" t="n">
-        <v>-1.636477884449312e-29</v>
+        <v>1.636477884449312e-29</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-1.069028481086101e-13</v>
+        <v>1.069028481086101e-13</v>
       </c>
       <c r="B2" t="n">
         <v>391.104</v>
@@ -1902,7 +1902,7 @@
         <v>6.545911537797249e-30</v>
       </c>
       <c r="D2" t="n">
-        <v>-977.76</v>
+        <v>977.76</v>
       </c>
       <c r="E2" t="n">
         <v>-2.672571202715251e-13</v>
@@ -1911,7 +1911,7 @@
         <v>5.987053271671581e-14</v>
       </c>
       <c r="G2" t="n">
-        <v>1.069028481086101e-13</v>
+        <v>-1.069028481086101e-13</v>
       </c>
       <c r="H2" t="n">
         <v>-391.104</v>
@@ -1920,7 +1920,7 @@
         <v>-6.545911537797249e-30</v>
       </c>
       <c r="J2" t="n">
-        <v>-977.76</v>
+        <v>977.76</v>
       </c>
       <c r="K2" t="n">
         <v>-2.672571202715251e-13</v>
@@ -1931,7 +1931,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>-1.282793029170869e-13</v>
+        <v>1.282793029170869e-13</v>
       </c>
       <c r="B3" t="n">
         <v>6.545911537797249e-30</v>
@@ -1940,7 +1940,7 @@
         <v>42</v>
       </c>
       <c r="D3" t="n">
-        <v>-1.636477884449312e-29</v>
+        <v>1.636477884449312e-29</v>
       </c>
       <c r="E3" t="n">
         <v>-3.27127652988241e-13</v>
@@ -1949,7 +1949,7 @@
         <v>1.002053701533141e-45</v>
       </c>
       <c r="G3" t="n">
-        <v>1.282793029170869e-13</v>
+        <v>-1.282793029170869e-13</v>
       </c>
       <c r="H3" t="n">
         <v>-6.545911537797249e-30</v>
@@ -1958,7 +1958,7 @@
         <v>-42</v>
       </c>
       <c r="J3" t="n">
-        <v>-1.636477884449312e-29</v>
+        <v>1.636477884449312e-29</v>
       </c>
       <c r="K3" t="n">
         <v>-3.27127652988241e-13</v>
@@ -1972,42 +1972,42 @@
         <v>2.672571202715251e-13</v>
       </c>
       <c r="B4" t="n">
-        <v>-977.76</v>
+        <v>977.76</v>
       </c>
       <c r="C4" t="n">
-        <v>-1.636477884449312e-29</v>
+        <v>1.636477884449312e-29</v>
       </c>
       <c r="D4" t="n">
         <v>3259.2</v>
       </c>
       <c r="E4" t="n">
-        <v>8.908570675717507e-13</v>
+        <v>-8.908570675717507e-13</v>
       </c>
       <c r="F4" t="n">
-        <v>-1.9759014794971e-13</v>
+        <v>1.9759014794971e-13</v>
       </c>
       <c r="G4" t="n">
         <v>-2.672571202715251e-13</v>
       </c>
       <c r="H4" t="n">
-        <v>977.76</v>
+        <v>-977.76</v>
       </c>
       <c r="I4" t="n">
-        <v>1.636477884449312e-29</v>
+        <v>-1.636477884449312e-29</v>
       </c>
       <c r="J4" t="n">
         <v>1629.6</v>
       </c>
       <c r="K4" t="n">
-        <v>4.454285337858754e-13</v>
+        <v>-4.454285337858754e-13</v>
       </c>
       <c r="L4" t="n">
-        <v>-1.01762515633869e-13</v>
+        <v>1.01762515633869e-13</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>5342.4</v>
+        <v>-5342.4</v>
       </c>
       <c r="B5" t="n">
         <v>-2.672571202715251e-13</v>
@@ -2016,7 +2016,7 @@
         <v>-3.27127652988241e-13</v>
       </c>
       <c r="D5" t="n">
-        <v>8.908570675717506e-13</v>
+        <v>-8.908570675717506e-13</v>
       </c>
       <c r="E5" t="n">
         <v>17808</v>
@@ -2025,7 +2025,7 @@
         <v>-5.454926281497708e-29</v>
       </c>
       <c r="G5" t="n">
-        <v>-5342.4</v>
+        <v>5342.4</v>
       </c>
       <c r="H5" t="n">
         <v>2.672571202715251e-13</v>
@@ -2034,7 +2034,7 @@
         <v>3.27127652988241e-13</v>
       </c>
       <c r="J5" t="n">
-        <v>4.454285337858753e-13</v>
+        <v>-4.454285337858753e-13</v>
       </c>
       <c r="K5" t="n">
         <v>8904</v>
@@ -2045,7 +2045,7 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-1.636477884449312e-29</v>
+        <v>1.636477884449312e-29</v>
       </c>
       <c r="B6" t="n">
         <v>5.987053271671581e-14</v>
@@ -2054,7 +2054,7 @@
         <v>1.002053701533141e-45</v>
       </c>
       <c r="D6" t="n">
-        <v>-1.9759014794971e-13</v>
+        <v>1.9759014794971e-13</v>
       </c>
       <c r="E6" t="n">
         <v>-5.454926281497709e-29</v>
@@ -2063,7 +2063,7 @@
         <v>32.308</v>
       </c>
       <c r="G6" t="n">
-        <v>1.636477884449312e-29</v>
+        <v>-1.636477884449312e-29</v>
       </c>
       <c r="H6" t="n">
         <v>-5.987053271671581e-14</v>
@@ -2072,7 +2072,7 @@
         <v>-1.002053701533141e-45</v>
       </c>
       <c r="J6" t="n">
-        <v>-1.01762515633869e-13</v>
+        <v>1.01762515633869e-13</v>
       </c>
       <c r="K6" t="n">
         <v>-2.727463140748855e-29</v>
@@ -2086,42 +2086,42 @@
         <v>-2136.96</v>
       </c>
       <c r="B7" t="n">
-        <v>1.069028481086101e-13</v>
+        <v>-1.069028481086101e-13</v>
       </c>
       <c r="C7" t="n">
-        <v>1.282793029170869e-13</v>
+        <v>-1.282793029170869e-13</v>
       </c>
       <c r="D7" t="n">
         <v>-2.672571202715251e-13</v>
       </c>
       <c r="E7" t="n">
-        <v>-5342.4</v>
+        <v>5342.4</v>
       </c>
       <c r="F7" t="n">
-        <v>1.636477884449312e-29</v>
+        <v>-1.636477884449312e-29</v>
       </c>
       <c r="G7" t="n">
         <v>2136.96</v>
       </c>
       <c r="H7" t="n">
-        <v>-1.069028481086101e-13</v>
+        <v>1.069028481086101e-13</v>
       </c>
       <c r="I7" t="n">
-        <v>-1.282793029170869e-13</v>
+        <v>1.282793029170869e-13</v>
       </c>
       <c r="J7" t="n">
         <v>-2.672571202715251e-13</v>
       </c>
       <c r="K7" t="n">
-        <v>-5342.4</v>
+        <v>5342.4</v>
       </c>
       <c r="L7" t="n">
-        <v>1.636477884449312e-29</v>
+        <v>-1.636477884449312e-29</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1.069028481086101e-13</v>
+        <v>-1.069028481086101e-13</v>
       </c>
       <c r="B8" t="n">
         <v>-391.104</v>
@@ -2130,7 +2130,7 @@
         <v>-6.545911537797249e-30</v>
       </c>
       <c r="D8" t="n">
-        <v>977.76</v>
+        <v>-977.76</v>
       </c>
       <c r="E8" t="n">
         <v>2.672571202715251e-13</v>
@@ -2139,7 +2139,7 @@
         <v>-5.987053271671581e-14</v>
       </c>
       <c r="G8" t="n">
-        <v>-1.069028481086101e-13</v>
+        <v>1.069028481086101e-13</v>
       </c>
       <c r="H8" t="n">
         <v>391.104</v>
@@ -2148,7 +2148,7 @@
         <v>6.545911537797249e-30</v>
       </c>
       <c r="J8" t="n">
-        <v>977.76</v>
+        <v>-977.76</v>
       </c>
       <c r="K8" t="n">
         <v>2.672571202715251e-13</v>
@@ -2159,7 +2159,7 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1.282793029170869e-13</v>
+        <v>-1.282793029170869e-13</v>
       </c>
       <c r="B9" t="n">
         <v>-6.545911537797249e-30</v>
@@ -2168,7 +2168,7 @@
         <v>-42</v>
       </c>
       <c r="D9" t="n">
-        <v>1.636477884449312e-29</v>
+        <v>-1.636477884449312e-29</v>
       </c>
       <c r="E9" t="n">
         <v>3.27127652988241e-13</v>
@@ -2177,7 +2177,7 @@
         <v>-1.002053701533141e-45</v>
       </c>
       <c r="G9" t="n">
-        <v>-1.282793029170869e-13</v>
+        <v>1.282793029170869e-13</v>
       </c>
       <c r="H9" t="n">
         <v>6.545911537797249e-30</v>
@@ -2186,7 +2186,7 @@
         <v>42</v>
       </c>
       <c r="J9" t="n">
-        <v>1.636477884449312e-29</v>
+        <v>-1.636477884449312e-29</v>
       </c>
       <c r="K9" t="n">
         <v>3.27127652988241e-13</v>
@@ -2200,42 +2200,42 @@
         <v>2.672571202715251e-13</v>
       </c>
       <c r="B10" t="n">
-        <v>-977.76</v>
+        <v>977.76</v>
       </c>
       <c r="C10" t="n">
-        <v>-1.636477884449312e-29</v>
+        <v>1.636477884449312e-29</v>
       </c>
       <c r="D10" t="n">
         <v>1629.6</v>
       </c>
       <c r="E10" t="n">
-        <v>4.454285337858754e-13</v>
+        <v>-4.454285337858754e-13</v>
       </c>
       <c r="F10" t="n">
-        <v>-1.01762515633869e-13</v>
+        <v>1.01762515633869e-13</v>
       </c>
       <c r="G10" t="n">
         <v>-2.672571202715251e-13</v>
       </c>
       <c r="H10" t="n">
-        <v>977.76</v>
+        <v>-977.76</v>
       </c>
       <c r="I10" t="n">
-        <v>1.636477884449312e-29</v>
+        <v>-1.636477884449312e-29</v>
       </c>
       <c r="J10" t="n">
         <v>3259.2</v>
       </c>
       <c r="K10" t="n">
-        <v>8.908570675717507e-13</v>
+        <v>-8.908570675717507e-13</v>
       </c>
       <c r="L10" t="n">
-        <v>-1.9759014794971e-13</v>
+        <v>1.9759014794971e-13</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>5342.4</v>
+        <v>-5342.4</v>
       </c>
       <c r="B11" t="n">
         <v>-2.672571202715251e-13</v>
@@ -2244,7 +2244,7 @@
         <v>-3.27127652988241e-13</v>
       </c>
       <c r="D11" t="n">
-        <v>4.454285337858753e-13</v>
+        <v>-4.454285337858753e-13</v>
       </c>
       <c r="E11" t="n">
         <v>8904</v>
@@ -2253,7 +2253,7 @@
         <v>-2.727463140748854e-29</v>
       </c>
       <c r="G11" t="n">
-        <v>-5342.4</v>
+        <v>5342.4</v>
       </c>
       <c r="H11" t="n">
         <v>2.672571202715251e-13</v>
@@ -2262,7 +2262,7 @@
         <v>3.27127652988241e-13</v>
       </c>
       <c r="J11" t="n">
-        <v>8.908570675717506e-13</v>
+        <v>-8.908570675717506e-13</v>
       </c>
       <c r="K11" t="n">
         <v>17808</v>
@@ -2273,7 +2273,7 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>-1.636477884449312e-29</v>
+        <v>1.636477884449312e-29</v>
       </c>
       <c r="B12" t="n">
         <v>5.987053271671581e-14</v>
@@ -2282,7 +2282,7 @@
         <v>1.002053701533141e-45</v>
       </c>
       <c r="D12" t="n">
-        <v>-1.01762515633869e-13</v>
+        <v>1.01762515633869e-13</v>
       </c>
       <c r="E12" t="n">
         <v>-2.727463140748855e-29</v>
@@ -2291,7 +2291,7 @@
         <v>-32.308</v>
       </c>
       <c r="G12" t="n">
-        <v>1.636477884449312e-29</v>
+        <v>-1.636477884449312e-29</v>
       </c>
       <c r="H12" t="n">
         <v>-5.987053271671581e-14</v>
@@ -2300,7 +2300,7 @@
         <v>-1.002053701533141e-45</v>
       </c>
       <c r="J12" t="n">
-        <v>-1.9759014794971e-13</v>
+        <v>1.9759014794971e-13</v>
       </c>
       <c r="K12" t="n">
         <v>-5.454926281497709e-29</v>
@@ -2333,37 +2333,37 @@
         <v>2136.96</v>
       </c>
       <c r="B1" t="n">
-        <v>-1.069028481086101e-13</v>
+        <v>1.069028481086101e-13</v>
       </c>
       <c r="C1" t="n">
-        <v>-1.282793029170869e-13</v>
+        <v>1.282793029170869e-13</v>
       </c>
       <c r="D1" t="n">
         <v>2.672571202715251e-13</v>
       </c>
       <c r="E1" t="n">
-        <v>5342.4</v>
+        <v>-5342.4</v>
       </c>
       <c r="F1" t="n">
-        <v>-1.636477884449312e-29</v>
+        <v>1.636477884449312e-29</v>
       </c>
       <c r="G1" t="n">
         <v>-2136.96</v>
       </c>
       <c r="H1" t="n">
-        <v>1.069028481086101e-13</v>
+        <v>-1.069028481086101e-13</v>
       </c>
       <c r="I1" t="n">
-        <v>1.282793029170869e-13</v>
+        <v>-1.282793029170869e-13</v>
       </c>
       <c r="J1" t="n">
         <v>2.672571202715251e-13</v>
       </c>
       <c r="K1" t="n">
-        <v>5342.4</v>
+        <v>-5342.4</v>
       </c>
       <c r="L1" t="n">
-        <v>-1.636477884449312e-29</v>
+        <v>1.636477884449312e-29</v>
       </c>
       <c r="M1" t="n">
         <v>0</v>
@@ -2404,7 +2404,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-1.069028481086101e-13</v>
+        <v>1.069028481086101e-13</v>
       </c>
       <c r="B2" t="n">
         <v>391.104</v>
@@ -2413,7 +2413,7 @@
         <v>6.545911537797249e-30</v>
       </c>
       <c r="D2" t="n">
-        <v>-977.76</v>
+        <v>977.76</v>
       </c>
       <c r="E2" t="n">
         <v>-2.672571202715251e-13</v>
@@ -2422,7 +2422,7 @@
         <v>5.987053271671581e-14</v>
       </c>
       <c r="G2" t="n">
-        <v>1.069028481086101e-13</v>
+        <v>-1.069028481086101e-13</v>
       </c>
       <c r="H2" t="n">
         <v>-391.104</v>
@@ -2431,7 +2431,7 @@
         <v>-6.545911537797249e-30</v>
       </c>
       <c r="J2" t="n">
-        <v>-977.76</v>
+        <v>977.76</v>
       </c>
       <c r="K2" t="n">
         <v>-2.672571202715251e-13</v>
@@ -2478,7 +2478,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>-1.282793029170869e-13</v>
+        <v>1.282793029170869e-13</v>
       </c>
       <c r="B3" t="n">
         <v>6.545911537797249e-30</v>
@@ -2487,7 +2487,7 @@
         <v>42</v>
       </c>
       <c r="D3" t="n">
-        <v>-1.636477884449312e-29</v>
+        <v>1.636477884449312e-29</v>
       </c>
       <c r="E3" t="n">
         <v>-3.27127652988241e-13</v>
@@ -2496,7 +2496,7 @@
         <v>1.002053701533141e-45</v>
       </c>
       <c r="G3" t="n">
-        <v>1.282793029170869e-13</v>
+        <v>-1.282793029170869e-13</v>
       </c>
       <c r="H3" t="n">
         <v>-6.545911537797249e-30</v>
@@ -2505,7 +2505,7 @@
         <v>-42</v>
       </c>
       <c r="J3" t="n">
-        <v>-1.636477884449312e-29</v>
+        <v>1.636477884449312e-29</v>
       </c>
       <c r="K3" t="n">
         <v>-3.27127652988241e-13</v>
@@ -2555,37 +2555,37 @@
         <v>2.672571202715251e-13</v>
       </c>
       <c r="B4" t="n">
-        <v>-977.76</v>
+        <v>977.76</v>
       </c>
       <c r="C4" t="n">
-        <v>-1.636477884449312e-29</v>
+        <v>1.636477884449312e-29</v>
       </c>
       <c r="D4" t="n">
         <v>3259.2</v>
       </c>
       <c r="E4" t="n">
-        <v>8.908570675717507e-13</v>
+        <v>-8.908570675717507e-13</v>
       </c>
       <c r="F4" t="n">
-        <v>-1.9759014794971e-13</v>
+        <v>1.9759014794971e-13</v>
       </c>
       <c r="G4" t="n">
         <v>-2.672571202715251e-13</v>
       </c>
       <c r="H4" t="n">
-        <v>977.76</v>
+        <v>-977.76</v>
       </c>
       <c r="I4" t="n">
-        <v>1.636477884449312e-29</v>
+        <v>-1.636477884449312e-29</v>
       </c>
       <c r="J4" t="n">
         <v>1629.6</v>
       </c>
       <c r="K4" t="n">
-        <v>4.454285337858754e-13</v>
+        <v>-4.454285337858754e-13</v>
       </c>
       <c r="L4" t="n">
-        <v>-1.01762515633869e-13</v>
+        <v>1.01762515633869e-13</v>
       </c>
       <c r="M4" t="n">
         <v>0</v>
@@ -2626,7 +2626,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>5342.4</v>
+        <v>-5342.4</v>
       </c>
       <c r="B5" t="n">
         <v>-2.672571202715251e-13</v>
@@ -2635,7 +2635,7 @@
         <v>-3.27127652988241e-13</v>
       </c>
       <c r="D5" t="n">
-        <v>8.908570675717506e-13</v>
+        <v>-8.908570675717506e-13</v>
       </c>
       <c r="E5" t="n">
         <v>17808</v>
@@ -2644,7 +2644,7 @@
         <v>-5.454926281497708e-29</v>
       </c>
       <c r="G5" t="n">
-        <v>-5342.4</v>
+        <v>5342.4</v>
       </c>
       <c r="H5" t="n">
         <v>2.672571202715251e-13</v>
@@ -2653,7 +2653,7 @@
         <v>3.27127652988241e-13</v>
       </c>
       <c r="J5" t="n">
-        <v>4.454285337858753e-13</v>
+        <v>-4.454285337858753e-13</v>
       </c>
       <c r="K5" t="n">
         <v>8904</v>
@@ -2700,7 +2700,7 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-1.636477884449312e-29</v>
+        <v>1.636477884449312e-29</v>
       </c>
       <c r="B6" t="n">
         <v>5.987053271671581e-14</v>
@@ -2709,7 +2709,7 @@
         <v>1.002053701533141e-45</v>
       </c>
       <c r="D6" t="n">
-        <v>-1.9759014794971e-13</v>
+        <v>1.9759014794971e-13</v>
       </c>
       <c r="E6" t="n">
         <v>-5.454926281497709e-29</v>
@@ -2718,7 +2718,7 @@
         <v>32.308</v>
       </c>
       <c r="G6" t="n">
-        <v>1.636477884449312e-29</v>
+        <v>-1.636477884449312e-29</v>
       </c>
       <c r="H6" t="n">
         <v>-5.987053271671581e-14</v>
@@ -2727,7 +2727,7 @@
         <v>-1.002053701533141e-45</v>
       </c>
       <c r="J6" t="n">
-        <v>-1.01762515633869e-13</v>
+        <v>1.01762515633869e-13</v>
       </c>
       <c r="K6" t="n">
         <v>-2.727463140748855e-29</v>
@@ -2777,37 +2777,37 @@
         <v>-2136.96</v>
       </c>
       <c r="B7" t="n">
-        <v>1.069028481086101e-13</v>
+        <v>-1.069028481086101e-13</v>
       </c>
       <c r="C7" t="n">
-        <v>1.282793029170869e-13</v>
+        <v>-1.282793029170869e-13</v>
       </c>
       <c r="D7" t="n">
         <v>-2.672571202715251e-13</v>
       </c>
       <c r="E7" t="n">
-        <v>-5342.4</v>
+        <v>5342.4</v>
       </c>
       <c r="F7" t="n">
-        <v>1.636477884449312e-29</v>
+        <v>-1.636477884449312e-29</v>
       </c>
       <c r="G7" t="n">
         <v>2157.96</v>
       </c>
       <c r="H7" t="n">
-        <v>-1.069028481086101e-13</v>
+        <v>1.069028481086101e-13</v>
       </c>
       <c r="I7" t="n">
-        <v>-1.282793029170869e-13</v>
+        <v>1.282793029170869e-13</v>
       </c>
       <c r="J7" t="n">
         <v>-2.672571202715251e-13</v>
       </c>
       <c r="K7" t="n">
-        <v>-5342.4</v>
+        <v>5342.4</v>
       </c>
       <c r="L7" t="n">
-        <v>1.636477884449312e-29</v>
+        <v>-1.636477884449312e-29</v>
       </c>
       <c r="M7" t="n">
         <v>-21</v>
@@ -2848,7 +2848,7 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1.069028481086101e-13</v>
+        <v>-1.069028481086101e-13</v>
       </c>
       <c r="B8" t="n">
         <v>-391.104</v>
@@ -2857,7 +2857,7 @@
         <v>-6.545911537797249e-30</v>
       </c>
       <c r="D8" t="n">
-        <v>977.76</v>
+        <v>-977.76</v>
       </c>
       <c r="E8" t="n">
         <v>2.672571202715251e-13</v>
@@ -2866,7 +2866,7 @@
         <v>-5.987053271671581e-14</v>
       </c>
       <c r="G8" t="n">
-        <v>-1.069028481086101e-13</v>
+        <v>1.069028481086101e-13</v>
       </c>
       <c r="H8" t="n">
         <v>439.992</v>
@@ -2875,7 +2875,7 @@
         <v>1.336285601357626e-14</v>
       </c>
       <c r="J8" t="n">
-        <v>977.76</v>
+        <v>-977.76</v>
       </c>
       <c r="K8" t="n">
         <v>2.004428402036438e-13</v>
@@ -2922,7 +2922,7 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1.282793029170869e-13</v>
+        <v>-1.282793029170869e-13</v>
       </c>
       <c r="B9" t="n">
         <v>-6.545911537797249e-30</v>
@@ -2931,7 +2931,7 @@
         <v>-42</v>
       </c>
       <c r="D9" t="n">
-        <v>1.636477884449312e-29</v>
+        <v>-1.636477884449312e-29</v>
       </c>
       <c r="E9" t="n">
         <v>3.27127652988241e-13</v>
@@ -2940,7 +2940,7 @@
         <v>-1.002053701533141e-45</v>
       </c>
       <c r="G9" t="n">
-        <v>-1.282793029170869e-13</v>
+        <v>1.282793029170869e-13</v>
       </c>
       <c r="H9" t="n">
         <v>1.336285601357626e-14</v>
@@ -2949,7 +2949,7 @@
         <v>309.12</v>
       </c>
       <c r="J9" t="n">
-        <v>1.636477884449312e-29</v>
+        <v>-1.636477884449312e-29</v>
       </c>
       <c r="K9" t="n">
         <v>-1335.6</v>
@@ -2999,37 +2999,37 @@
         <v>2.672571202715251e-13</v>
       </c>
       <c r="B10" t="n">
-        <v>-977.76</v>
+        <v>977.76</v>
       </c>
       <c r="C10" t="n">
-        <v>-1.636477884449312e-29</v>
+        <v>1.636477884449312e-29</v>
       </c>
       <c r="D10" t="n">
         <v>1629.6</v>
       </c>
       <c r="E10" t="n">
-        <v>4.454285337858754e-13</v>
+        <v>-4.454285337858754e-13</v>
       </c>
       <c r="F10" t="n">
-        <v>-1.01762515633869e-13</v>
+        <v>1.01762515633869e-13</v>
       </c>
       <c r="G10" t="n">
         <v>-2.672571202715251e-13</v>
       </c>
       <c r="H10" t="n">
-        <v>977.76</v>
+        <v>-977.76</v>
       </c>
       <c r="I10" t="n">
-        <v>1.636477884449312e-29</v>
+        <v>-1.636477884449312e-29</v>
       </c>
       <c r="J10" t="n">
         <v>3275.354</v>
       </c>
       <c r="K10" t="n">
-        <v>8.908570675717507e-13</v>
+        <v>-8.908570675717507e-13</v>
       </c>
       <c r="L10" t="n">
-        <v>-1.9759014794971e-13</v>
+        <v>1.9759014794971e-13</v>
       </c>
       <c r="M10" t="n">
         <v>0</v>
@@ -3070,7 +3070,7 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>5342.4</v>
+        <v>-5342.4</v>
       </c>
       <c r="B11" t="n">
         <v>-2.672571202715251e-13</v>
@@ -3079,7 +3079,7 @@
         <v>-3.27127652988241e-13</v>
       </c>
       <c r="D11" t="n">
-        <v>4.454285337858753e-13</v>
+        <v>-4.454285337858753e-13</v>
       </c>
       <c r="E11" t="n">
         <v>8904</v>
@@ -3088,7 +3088,7 @@
         <v>-2.727463140748854e-29</v>
       </c>
       <c r="G11" t="n">
-        <v>-5342.4</v>
+        <v>5342.4</v>
       </c>
       <c r="H11" t="n">
         <v>2.004428402036438e-13</v>
@@ -3097,7 +3097,7 @@
         <v>-1335.6</v>
       </c>
       <c r="J11" t="n">
-        <v>8.908570675717506e-13</v>
+        <v>-8.908570675717506e-13</v>
       </c>
       <c r="K11" t="n">
         <v>26712</v>
@@ -3144,7 +3144,7 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>-1.636477884449312e-29</v>
+        <v>1.636477884449312e-29</v>
       </c>
       <c r="B12" t="n">
         <v>5.987053271671581e-14</v>
@@ -3153,7 +3153,7 @@
         <v>1.002053701533141e-45</v>
       </c>
       <c r="D12" t="n">
-        <v>-1.01762515633869e-13</v>
+        <v>1.01762515633869e-13</v>
       </c>
       <c r="E12" t="n">
         <v>-2.727463140748855e-29</v>
@@ -3162,7 +3162,7 @@
         <v>-32.308</v>
       </c>
       <c r="G12" t="n">
-        <v>1.636477884449312e-29</v>
+        <v>-1.636477884449312e-29</v>
       </c>
       <c r="H12" t="n">
         <v>244.4399999999999</v>
@@ -3171,7 +3171,7 @@
         <v>6.681428006788129e-14</v>
       </c>
       <c r="J12" t="n">
-        <v>-1.9759014794971e-13</v>
+        <v>1.9759014794971e-13</v>
       </c>
       <c r="K12" t="n">
         <v>-4.454285337858754e-13</v>
@@ -3260,13 +3260,13 @@
         <v>0</v>
       </c>
       <c r="O13" t="n">
-        <v>2.137645480847688e-14</v>
+        <v>-2.137645480847688e-14</v>
       </c>
       <c r="P13" t="n">
         <v>0</v>
       </c>
       <c r="Q13" t="n">
-        <v>-977.76</v>
+        <v>977.76</v>
       </c>
       <c r="R13" t="n">
         <v>0</v>
@@ -3278,13 +3278,13 @@
         <v>0</v>
       </c>
       <c r="U13" t="n">
-        <v>-2.137645480847688e-14</v>
+        <v>2.137645480847688e-14</v>
       </c>
       <c r="V13" t="n">
         <v>0</v>
       </c>
       <c r="W13" t="n">
-        <v>-977.76</v>
+        <v>977.76</v>
       </c>
       <c r="X13" t="n">
         <v>0</v>
@@ -3337,7 +3337,7 @@
         <v>1.336285601357626e-14</v>
       </c>
       <c r="P14" t="n">
-        <v>5342.4</v>
+        <v>-5342.4</v>
       </c>
       <c r="Q14" t="n">
         <v>6.681428006788129e-14</v>
@@ -3355,7 +3355,7 @@
         <v>0</v>
       </c>
       <c r="V14" t="n">
-        <v>5342.4</v>
+        <v>-5342.4</v>
       </c>
       <c r="W14" t="n">
         <v>0</v>
@@ -3402,7 +3402,7 @@
         <v>-6.681428006788129e-14</v>
       </c>
       <c r="M15" t="n">
-        <v>2.137645480847688e-14</v>
+        <v>-2.137645480847688e-14</v>
       </c>
       <c r="N15" t="n">
         <v>1.336285601357626e-14</v>
@@ -3420,7 +3420,7 @@
         <v>-6.681428006788129e-14</v>
       </c>
       <c r="S15" t="n">
-        <v>-2.137645480847688e-14</v>
+        <v>2.137645480847688e-14</v>
       </c>
       <c r="T15" t="n">
         <v>0</v>
@@ -3479,7 +3479,7 @@
         <v>0</v>
       </c>
       <c r="N16" t="n">
-        <v>5342.4</v>
+        <v>-5342.4</v>
       </c>
       <c r="O16" t="n">
         <v>0</v>
@@ -3491,13 +3491,13 @@
         <v>0</v>
       </c>
       <c r="R16" t="n">
-        <v>1.088447215521461e-12</v>
+        <v>-1.088447215521461e-12</v>
       </c>
       <c r="S16" t="n">
         <v>0</v>
       </c>
       <c r="T16" t="n">
-        <v>-5342.4</v>
+        <v>5342.4</v>
       </c>
       <c r="U16" t="n">
         <v>0</v>
@@ -3509,7 +3509,7 @@
         <v>0</v>
       </c>
       <c r="X16" t="n">
-        <v>5.471910494197443e-13</v>
+        <v>-5.471910494197443e-13</v>
       </c>
     </row>
     <row r="17">
@@ -3550,7 +3550,7 @@
         <v>-2.227142668929377e-13</v>
       </c>
       <c r="M17" t="n">
-        <v>-977.76</v>
+        <v>977.76</v>
       </c>
       <c r="N17" t="n">
         <v>6.681428006788129e-14</v>
@@ -3568,7 +3568,7 @@
         <v>-4.454285337858753e-13</v>
       </c>
       <c r="S17" t="n">
-        <v>977.76</v>
+        <v>-977.76</v>
       </c>
       <c r="T17" t="n">
         <v>0</v>
@@ -3633,7 +3633,7 @@
         <v>-6.681428006788129e-14</v>
       </c>
       <c r="P18" t="n">
-        <v>1.088447215521461e-12</v>
+        <v>-1.088447215521461e-12</v>
       </c>
       <c r="Q18" t="n">
         <v>-4.454285337858754e-13</v>
@@ -3651,7 +3651,7 @@
         <v>0</v>
       </c>
       <c r="V18" t="n">
-        <v>5.471910494197443e-13</v>
+        <v>-5.471910494197443e-13</v>
       </c>
       <c r="W18" t="n">
         <v>0</v>
@@ -3704,13 +3704,13 @@
         <v>0</v>
       </c>
       <c r="O19" t="n">
-        <v>-2.137645480847688e-14</v>
+        <v>2.137645480847688e-14</v>
       </c>
       <c r="P19" t="n">
         <v>0</v>
       </c>
       <c r="Q19" t="n">
-        <v>977.76</v>
+        <v>-977.76</v>
       </c>
       <c r="R19" t="n">
         <v>0</v>
@@ -3722,13 +3722,13 @@
         <v>0</v>
       </c>
       <c r="U19" t="n">
-        <v>2.137645480847688e-14</v>
+        <v>-2.137645480847688e-14</v>
       </c>
       <c r="V19" t="n">
         <v>0</v>
       </c>
       <c r="W19" t="n">
-        <v>977.76</v>
+        <v>-977.76</v>
       </c>
       <c r="X19" t="n">
         <v>0</v>
@@ -3781,7 +3781,7 @@
         <v>0</v>
       </c>
       <c r="P20" t="n">
-        <v>-5342.4</v>
+        <v>5342.4</v>
       </c>
       <c r="Q20" t="n">
         <v>0</v>
@@ -3799,7 +3799,7 @@
         <v>0</v>
       </c>
       <c r="V20" t="n">
-        <v>-5342.4</v>
+        <v>5342.4</v>
       </c>
       <c r="W20" t="n">
         <v>0</v>
@@ -3846,7 +3846,7 @@
         <v>0</v>
       </c>
       <c r="M21" t="n">
-        <v>-2.137645480847688e-14</v>
+        <v>2.137645480847688e-14</v>
       </c>
       <c r="N21" t="n">
         <v>0</v>
@@ -3864,7 +3864,7 @@
         <v>0</v>
       </c>
       <c r="S21" t="n">
-        <v>2.137645480847688e-14</v>
+        <v>-2.137645480847688e-14</v>
       </c>
       <c r="T21" t="n">
         <v>0</v>
@@ -3923,7 +3923,7 @@
         <v>0</v>
       </c>
       <c r="N22" t="n">
-        <v>5342.4</v>
+        <v>-5342.4</v>
       </c>
       <c r="O22" t="n">
         <v>0</v>
@@ -3935,13 +3935,13 @@
         <v>0</v>
       </c>
       <c r="R22" t="n">
-        <v>5.471910494197443e-13</v>
+        <v>-5.471910494197443e-13</v>
       </c>
       <c r="S22" t="n">
         <v>0</v>
       </c>
       <c r="T22" t="n">
-        <v>-5342.4</v>
+        <v>5342.4</v>
       </c>
       <c r="U22" t="n">
         <v>0</v>
@@ -3953,7 +3953,7 @@
         <v>0</v>
       </c>
       <c r="X22" t="n">
-        <v>1.088447215521461e-12</v>
+        <v>-1.088447215521461e-12</v>
       </c>
     </row>
     <row r="23">
@@ -3994,7 +3994,7 @@
         <v>0</v>
       </c>
       <c r="M23" t="n">
-        <v>-977.76</v>
+        <v>977.76</v>
       </c>
       <c r="N23" t="n">
         <v>0</v>
@@ -4012,7 +4012,7 @@
         <v>0</v>
       </c>
       <c r="S23" t="n">
-        <v>977.76</v>
+        <v>-977.76</v>
       </c>
       <c r="T23" t="n">
         <v>0</v>
@@ -4077,7 +4077,7 @@
         <v>0</v>
       </c>
       <c r="P24" t="n">
-        <v>5.471910494197443e-13</v>
+        <v>-5.471910494197443e-13</v>
       </c>
       <c r="Q24" t="n">
         <v>0</v>
@@ -4095,7 +4095,7 @@
         <v>0</v>
       </c>
       <c r="V24" t="n">
-        <v>1.088447215521461e-12</v>
+        <v>-1.088447215521461e-12</v>
       </c>
       <c r="W24" t="n">
         <v>0</v>
@@ -4125,122 +4125,122 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>-1.75973421993209</v>
+        <v>2.748314368632023e-16</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-1.523852505115035e-16</v>
+        <v>1.75973421993209</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1.999697977195557</v>
+        <v>-1.999697977195557</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2.077980688793229e-16</v>
+        <v>2.399637572634668</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>-2.399637572634668</v>
+        <v>-2.077980688793229e-16</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-1.27239619961032e-32</v>
+        <v>1.469354236220385e-16</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>-3.239510723056802</v>
+        <v>-3.5</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>-2.805273929870859e-16</v>
+        <v>3.239510723056801</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>2.999546965793335</v>
+        <v>-14.51664747064227</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>-3.116971033189843e-16</v>
+        <v>-3.599456358952002</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>3.599456358952002</v>
+        <v>20.30570230503482</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>1.90859429941548e-32</v>
+        <v>-1.56139138049941e-15</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>0</v>
+        <v>-0.5199214740708445</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0</v>
+        <v>2.51725151625115</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>0</v>
+        <v>0.7998791908782228</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>0</v>
+        <v>-5.756475521456251</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>0</v>
+        <v>2.633064592418956e-16</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>0</v>
+        <v>-6.327821012781338e-16</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>0</v>
+        <v>-4.479323468918047</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>0</v>
+        <v>-3.999395954391114</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>0</v>
+        <v>-3.199516763512891</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>0</v>
+        <v>2.770640918390973e-16</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>0</v>
+        <v>1.959138981627181e-16</v>
       </c>
     </row>
   </sheetData>
@@ -4294,62 +4294,62 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.0009119937728235471</v>
+        <v>0.01380814379189671</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>-1.649334516455838e-18</v>
+        <v>0.02167331059878497</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.04601165711126328</v>
+        <v>-0.2126831458241319</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>2.125535289402686e-19</v>
+        <v>0.00537055645510233</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0.0009524767042113616</v>
+        <v>-0.006031248225553358</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>-1.315386607524273e-19</v>
+        <v>-0.002183288066494276</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0.005668821927634335</v>
+        <v>0.05124197414119706</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>-2.581699923940913e-21</v>
+        <v>-0.0004481385117980237</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0.02540612778857801</v>
+        <v>-0.07301675785184697</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>9.664449364700713e-22</v>
+        <v>-8.457624555846062e-05</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>0.002369694324206886</v>
+        <v>-0.01772117031976563</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>2.410638683997671e-19</v>
+        <v>-0.002183288066494276</v>
       </c>
     </row>
     <row r="19">
@@ -4403,116 +4403,116 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>4.899351551737866</v>
+        <v>2.713889562664689</v>
       </c>
       <c r="B1" t="n">
-        <v>4.325587894577225e-16</v>
+        <v>-4.985137408818432</v>
       </c>
       <c r="C1" t="n">
-        <v>-3.932187575868615</v>
+        <v>10.9323901018091</v>
       </c>
       <c r="D1" t="n">
-        <v>-1.293550682536436e-15</v>
+        <v>-14.8390749444679</v>
       </c>
       <c r="E1" t="n">
-        <v>6.00825461500013</v>
+        <v>20.06639319350182</v>
       </c>
       <c r="F1" t="n">
-        <v>4.249751051589502e-18</v>
+        <v>0.07053767085229616</v>
       </c>
       <c r="G1" t="n">
-        <v>0.09989339125102514</v>
+        <v>-2.71388956266469</v>
       </c>
       <c r="H1" t="n">
-        <v>3.538540408669117e-19</v>
+        <v>-0.01410753417045951</v>
       </c>
       <c r="I1" t="n">
-        <v>-1.067057367120277</v>
+        <v>-5.933145158820207</v>
       </c>
       <c r="J1" t="n">
-        <v>-3.417977754997201e-18</v>
+        <v>-0.08812221364647188</v>
       </c>
       <c r="K1" t="n">
-        <v>8.490013257711421</v>
+        <v>-33.63584100682528</v>
       </c>
       <c r="L1" t="n">
-        <v>-4.249751051589422e-18</v>
+        <v>-0.07053767085229709</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-0.09989339125102654</v>
+        <v>2.713889562664693</v>
       </c>
       <c r="B2" t="n">
-        <v>-3.538540408669117e-19</v>
+        <v>0.01410753417046012</v>
       </c>
       <c r="C2" t="n">
-        <v>1.067057367120276</v>
+        <v>5.933145158820203</v>
       </c>
       <c r="D2" t="n">
-        <v>3.417977754997361e-18</v>
+        <v>0.08812221364647442</v>
       </c>
       <c r="E2" t="n">
-        <v>-8.490013257711418</v>
+        <v>33.63584100682527</v>
       </c>
       <c r="F2" t="n">
-        <v>4.249751051589763e-18</v>
+        <v>0.07053767085229688</v>
       </c>
       <c r="G2" t="n">
-        <v>0.09989339125102654</v>
+        <v>-2.713889562664693</v>
       </c>
       <c r="H2" t="n">
-        <v>3.538540408669117e-19</v>
+        <v>-0.01410753417045963</v>
       </c>
       <c r="I2" t="n">
-        <v>-1.067057367120276</v>
+        <v>2.066854841179799</v>
       </c>
       <c r="J2" t="n">
-        <v>-3.417977754997361e-18</v>
+        <v>-0.08812221364647442</v>
       </c>
       <c r="K2" t="n">
-        <v>-2.180560413491335</v>
+        <v>7.654485669883327</v>
       </c>
       <c r="L2" t="n">
-        <v>-7.788291460259669e-18</v>
+        <v>0.07053767085229759</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>-0.09989339125102581</v>
+        <v>2.713889562664697</v>
       </c>
       <c r="B3" t="n">
-        <v>-3.538540408669856e-19</v>
+        <v>0.01410753417045951</v>
       </c>
       <c r="C3" t="n">
-        <v>1.067057367120277</v>
+        <v>-2.066854841179794</v>
       </c>
       <c r="D3" t="n">
-        <v>3.417977754997361e-18</v>
+        <v>0.08812221364647432</v>
       </c>
       <c r="E3" t="n">
-        <v>2.180560413491336</v>
+        <v>-7.654485669883286</v>
       </c>
       <c r="F3" t="n">
-        <v>7.788291460259675e-18</v>
+        <v>-0.07053767085229706</v>
       </c>
       <c r="G3" t="n">
-        <v>0.09989339125102581</v>
+        <v>-2.713889562664697</v>
       </c>
       <c r="H3" t="n">
-        <v>3.538540408669856e-19</v>
+        <v>4.985137408818433</v>
       </c>
       <c r="I3" t="n">
-        <v>-1.067057367120277</v>
+        <v>7.066099784168687</v>
       </c>
       <c r="J3" t="n">
-        <v>-5.187247959332283e-18</v>
+        <v>4.84058505849012</v>
       </c>
       <c r="K3" t="n">
-        <v>-1.681093457236207</v>
+        <v>21.22393348320678</v>
       </c>
       <c r="L3" t="n">
-        <v>-7.788291460259677e-18</v>
+        <v>0.07053767085229677</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add nodal loads and update bar transformation logic
Introduces support for nodal loads in the structure assembly and updates the transformation logic for bar reactions and stiffness matrices. Modifies test data in Prueba_1.py to use new nodal loads and revised geometry, and adds additional output to the Excel export. Also adds a new attribute to Nodo for global reactions.
</commit_message>
<xml_diff>
--- a/matrices_rigidez_3D.xlsx
+++ b/matrices_rigidez_3D.xlsx
@@ -8,11 +8,15 @@
   </bookViews>
   <sheets>
     <sheet name="Barra 1 (K1local)" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Barra 1 (K1)" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Global" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="F" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Desplazamientos" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Reacciones" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Barra 2 (K2local)" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Barra 3 (K3local)" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Barra 1 (K1)" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Barra 2 (K2)" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Barra 3 (K3)" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Global" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="F" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Desplazamientos" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="Reacciones" sheetId="10" state="visible" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -428,7 +432,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>2</v>
+        <v>0.02</v>
       </c>
       <c r="B1" t="n">
         <v>0</v>
@@ -446,7 +450,7 @@
         <v>0</v>
       </c>
       <c r="G1" t="n">
-        <v>-2</v>
+        <v>-0.02</v>
       </c>
       <c r="H1" t="n">
         <v>0</v>
@@ -469,7 +473,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>9.6</v>
+        <v>0.00096</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -481,13 +485,13 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>24</v>
+        <v>0.24</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>-9.6</v>
+        <v>-0.00096</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -499,7 +503,7 @@
         <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>24</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="3">
@@ -510,13 +514,13 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>9.6</v>
+        <v>0.1152</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>-24</v>
+        <v>-28.8</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
@@ -528,13 +532,13 @@
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>-9.6</v>
+        <v>-0.1152</v>
       </c>
       <c r="J3" t="n">
         <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>-24</v>
+        <v>-28.8</v>
       </c>
       <c r="L3" t="n">
         <v>0</v>
@@ -551,7 +555,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>32.308</v>
+        <v>0.32308</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -569,7 +573,7 @@
         <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>-32.308</v>
+        <v>-0.32308</v>
       </c>
       <c r="K4" t="n">
         <v>0</v>
@@ -586,13 +590,13 @@
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>-24</v>
+        <v>-28.8</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>80</v>
+        <v>9600</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
@@ -604,13 +608,13 @@
         <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>24</v>
+        <v>28.8</v>
       </c>
       <c r="J5" t="n">
         <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>40</v>
+        <v>4800</v>
       </c>
       <c r="L5" t="n">
         <v>0</v>
@@ -621,7 +625,7 @@
         <v>0</v>
       </c>
       <c r="B6" t="n">
-        <v>24</v>
+        <v>0.24</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
@@ -639,7 +643,7 @@
         <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>-24</v>
+        <v>-0.24</v>
       </c>
       <c r="I6" t="n">
         <v>0</v>
@@ -656,7 +660,7 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>-2</v>
+        <v>-0.02</v>
       </c>
       <c r="B7" t="n">
         <v>0</v>
@@ -674,7 +678,7 @@
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>2</v>
+        <v>0.02</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -697,7 +701,7 @@
         <v>0</v>
       </c>
       <c r="B8" t="n">
-        <v>-9.6</v>
+        <v>-0.00096</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
@@ -709,13 +713,13 @@
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>-24</v>
+        <v>-0.24</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>9.6</v>
+        <v>0.00096</v>
       </c>
       <c r="I8" t="n">
         <v>0</v>
@@ -727,7 +731,7 @@
         <v>0</v>
       </c>
       <c r="L8" t="n">
-        <v>-24</v>
+        <v>-0.24</v>
       </c>
     </row>
     <row r="9">
@@ -738,13 +742,13 @@
         <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>-9.6</v>
+        <v>-0.1152</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>24</v>
+        <v>28.8</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
@@ -756,13 +760,13 @@
         <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>9.6</v>
+        <v>0.1152</v>
       </c>
       <c r="J9" t="n">
         <v>0</v>
       </c>
       <c r="K9" t="n">
-        <v>24</v>
+        <v>28.8</v>
       </c>
       <c r="L9" t="n">
         <v>0</v>
@@ -779,7 +783,7 @@
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>-32.308</v>
+        <v>-0.32308</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
@@ -797,7 +801,7 @@
         <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>32.308</v>
+        <v>0.32308</v>
       </c>
       <c r="K10" t="n">
         <v>0</v>
@@ -814,13 +818,13 @@
         <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>-24</v>
+        <v>-28.8</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>40</v>
+        <v>4800</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
@@ -832,13 +836,13 @@
         <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>24</v>
+        <v>28.8</v>
       </c>
       <c r="J11" t="n">
         <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>80</v>
+        <v>9600</v>
       </c>
       <c r="L11" t="n">
         <v>0</v>
@@ -849,7 +853,7 @@
         <v>0</v>
       </c>
       <c r="B12" t="n">
-        <v>24</v>
+        <v>0.24</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
@@ -867,7 +871,7 @@
         <v>0</v>
       </c>
       <c r="H12" t="n">
-        <v>-24</v>
+        <v>-0.24</v>
       </c>
       <c r="I12" t="n">
         <v>0</v>
@@ -880,6 +884,139 @@
       </c>
       <c r="L12" t="n">
         <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="n">
+        <v>-0.2018676928313105</v>
+      </c>
+      <c r="B1" t="n">
+        <v>0.5444187525595298</v>
+      </c>
+      <c r="C1" t="n">
+        <v>2.414857899806747e-17</v>
+      </c>
+      <c r="D1" t="n">
+        <v>2.072827630792632e-14</v>
+      </c>
+      <c r="E1" t="n">
+        <v>-1.934518200724968e-16</v>
+      </c>
+      <c r="F1" t="n">
+        <v>29.70218384172761</v>
+      </c>
+      <c r="G1" t="n">
+        <v>-0.2980568014675786</v>
+      </c>
+      <c r="H1" t="n">
+        <v>-1.044343246858419</v>
+      </c>
+      <c r="I1" t="n">
+        <v>-6.743984334792639e-17</v>
+      </c>
+      <c r="J1" t="n">
+        <v>4.26606107920184e-18</v>
+      </c>
+      <c r="K1" t="n">
+        <v>1.934518200724968e-16</v>
+      </c>
+      <c r="L1" t="n">
+        <v>-28.7532362858502</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>0.2980568014675774</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1.044343246858419</v>
+      </c>
+      <c r="C2" t="n">
+        <v>6.743984334792499e-17</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-4.266061079206575e-18</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-1.934518200724858e-16</v>
+      </c>
+      <c r="F2" t="n">
+        <v>128.7532362858502</v>
+      </c>
+      <c r="G2" t="n">
+        <v>-0.2980568014675774</v>
+      </c>
+      <c r="H2" t="n">
+        <v>-0.2443432468584192</v>
+      </c>
+      <c r="I2" t="n">
+        <v>-1.845397138203085e-17</v>
+      </c>
+      <c r="J2" t="n">
+        <v>4.266061079206575e-18</v>
+      </c>
+      <c r="K2" t="n">
+        <v>1.091824252519305e-16</v>
+      </c>
+      <c r="L2" t="n">
+        <v>-90.62777207653821</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>0.2980568014675786</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.244343246858419</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1.845397138203069e-17</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-4.266061079199769e-18</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-1.091824252519212e-16</v>
+      </c>
+      <c r="F3" t="n">
+        <v>90.62777207653824</v>
+      </c>
+      <c r="G3" t="n">
+        <v>-0.7979812957664678</v>
+      </c>
+      <c r="H3" t="n">
+        <v>-0.7442677411573082</v>
+      </c>
+      <c r="I3" t="n">
+        <v>-6.174523573188963e-17</v>
+      </c>
+      <c r="J3" t="n">
+        <v>-1.355184606492203e-14</v>
+      </c>
+      <c r="K3" t="n">
+        <v>1.091824252519212e-16</v>
+      </c>
+      <c r="L3" t="n">
+        <v>108.39307808714</v>
       </c>
     </row>
   </sheetData>
@@ -903,7 +1040,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>9.6</v>
+        <v>0.01</v>
       </c>
       <c r="B1" t="n">
         <v>0</v>
@@ -918,10 +1055,10 @@
         <v>0</v>
       </c>
       <c r="F1" t="n">
-        <v>-24</v>
+        <v>0</v>
       </c>
       <c r="G1" t="n">
-        <v>-9.6</v>
+        <v>-0.01</v>
       </c>
       <c r="H1" t="n">
         <v>0</v>
@@ -936,7 +1073,7 @@
         <v>0</v>
       </c>
       <c r="L1" t="n">
-        <v>-24</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2">
@@ -944,7 +1081,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>0.00012</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -956,13 +1093,13 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>0.06</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>-2</v>
+        <v>-0.00012</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -974,7 +1111,7 @@
         <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="3">
@@ -985,13 +1122,13 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>9.6</v>
+        <v>0.0144</v>
       </c>
       <c r="D3" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>-7.2</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
@@ -1003,13 +1140,13 @@
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>-9.6</v>
+        <v>-0.0144</v>
       </c>
       <c r="J3" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>-7.2</v>
       </c>
       <c r="L3" t="n">
         <v>0</v>
@@ -1023,10 +1160,10 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>80</v>
+        <v>0.16154</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -1041,10 +1178,10 @@
         <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>-24</v>
+        <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>40</v>
+        <v>-0.16154</v>
       </c>
       <c r="K4" t="n">
         <v>0</v>
@@ -1061,13 +1198,13 @@
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>-7.2</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>32.308</v>
+        <v>4800</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
@@ -1079,13 +1216,13 @@
         <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>7.2</v>
       </c>
       <c r="J5" t="n">
         <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>-32.308</v>
+        <v>2400</v>
       </c>
       <c r="L5" t="n">
         <v>0</v>
@@ -1093,10 +1230,10 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-24</v>
+        <v>0</v>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>0.06</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
@@ -1108,13 +1245,13 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="G6" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>-0.06</v>
       </c>
       <c r="I6" t="n">
         <v>0</v>
@@ -1126,12 +1263,12 @@
         <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>-9.6</v>
+        <v>-0.01</v>
       </c>
       <c r="B7" t="n">
         <v>0</v>
@@ -1146,10 +1283,10 @@
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>9.6</v>
+        <v>0.01</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -1164,7 +1301,7 @@
         <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -1172,7 +1309,7 @@
         <v>0</v>
       </c>
       <c r="B8" t="n">
-        <v>-2</v>
+        <v>-0.00012</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
@@ -1184,13 +1321,13 @@
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>-0.06</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>2</v>
+        <v>0.00012</v>
       </c>
       <c r="I8" t="n">
         <v>0</v>
@@ -1202,7 +1339,7 @@
         <v>0</v>
       </c>
       <c r="L8" t="n">
-        <v>0</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="9">
@@ -1213,13 +1350,13 @@
         <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>-9.6</v>
+        <v>-0.0144</v>
       </c>
       <c r="D9" t="n">
-        <v>-24</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>7.2</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
@@ -1231,13 +1368,13 @@
         <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>9.6</v>
+        <v>0.0144</v>
       </c>
       <c r="J9" t="n">
-        <v>-24</v>
+        <v>0</v>
       </c>
       <c r="K9" t="n">
-        <v>0</v>
+        <v>7.2</v>
       </c>
       <c r="L9" t="n">
         <v>0</v>
@@ -1251,10 +1388,10 @@
         <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>40</v>
+        <v>-0.16154</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
@@ -1269,10 +1406,10 @@
         <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>-24</v>
+        <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>80</v>
+        <v>0.16154</v>
       </c>
       <c r="K10" t="n">
         <v>0</v>
@@ -1289,13 +1426,13 @@
         <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>-7.2</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>-32.308</v>
+        <v>2400</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
@@ -1307,13 +1444,13 @@
         <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>7.2</v>
       </c>
       <c r="J11" t="n">
         <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>32.308</v>
+        <v>4800</v>
       </c>
       <c r="L11" t="n">
         <v>0</v>
@@ -1321,10 +1458,10 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>-24</v>
+        <v>0</v>
       </c>
       <c r="B12" t="n">
-        <v>0</v>
+        <v>0.06</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
@@ -1336,25 +1473,25 @@
         <v>0</v>
       </c>
       <c r="F12" t="n">
+        <v>20</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>-0.06</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="n">
         <v>40</v>
-      </c>
-      <c r="G12" t="n">
-        <v>24</v>
-      </c>
-      <c r="H12" t="n">
-        <v>0</v>
-      </c>
-      <c r="I12" t="n">
-        <v>0</v>
-      </c>
-      <c r="J12" t="n">
-        <v>0</v>
-      </c>
-      <c r="K12" t="n">
-        <v>0</v>
-      </c>
-      <c r="L12" t="n">
-        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1363,6 +1500,1906 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="B1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G1" t="n">
+        <v>-0.02</v>
+      </c>
+      <c r="H1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.009599999999999999</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>-0.009599999999999999</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>0</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.01152</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-2.88</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>-0.01152</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>-2.88</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>0</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.32308</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>-0.32308</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>0</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-2.88</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>960</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>2.88</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>480</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>0</v>
+      </c>
+      <c r="B6" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>800</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>-2.4</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>-0.02</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>0</v>
+      </c>
+      <c r="B8" t="n">
+        <v>-0.009599999999999999</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-2.4</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.009599999999999999</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>-2.4</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>0</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>-0.01152</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>2.88</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.01152</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>2.88</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>0</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>-0.32308</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.32308</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>0</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>-2.88</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>480</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>2.88</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>960</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>0</v>
+      </c>
+      <c r="B12" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>400</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>-2.4</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>800</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="n">
+        <v>0.00096</v>
+      </c>
+      <c r="B1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F1" t="n">
+        <v>-0.24</v>
+      </c>
+      <c r="G1" t="n">
+        <v>-0.00096</v>
+      </c>
+      <c r="H1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L1" t="n">
+        <v>-0.24</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>-0.02</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>0</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.1152</v>
+      </c>
+      <c r="D3" t="n">
+        <v>28.8</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>-0.1152</v>
+      </c>
+      <c r="J3" t="n">
+        <v>28.8</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>0</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>28.8</v>
+      </c>
+      <c r="D4" t="n">
+        <v>9600</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>-28.8</v>
+      </c>
+      <c r="J4" t="n">
+        <v>4800</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>0</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.32308</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>-0.32308</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>-0.24</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>80</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>-0.00096</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.00096</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>0</v>
+      </c>
+      <c r="B8" t="n">
+        <v>-0.02</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>0</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>-0.1152</v>
+      </c>
+      <c r="D9" t="n">
+        <v>-28.8</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.1152</v>
+      </c>
+      <c r="J9" t="n">
+        <v>-28.8</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>0</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>28.8</v>
+      </c>
+      <c r="D10" t="n">
+        <v>4800</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>-28.8</v>
+      </c>
+      <c r="J10" t="n">
+        <v>9600</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>0</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-0.32308</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.32308</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>-0.24</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>40</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="B1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G1" t="n">
+        <v>-0.01</v>
+      </c>
+      <c r="H1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.0144</v>
+      </c>
+      <c r="C2" t="n">
+        <v>-8.743978145912101e-19</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>4.371989072956051e-16</v>
+      </c>
+      <c r="F2" t="n">
+        <v>7.2</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>-0.0144</v>
+      </c>
+      <c r="I2" t="n">
+        <v>8.743978145912101e-19</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>4.371989072956051e-16</v>
+      </c>
+      <c r="L2" t="n">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>0</v>
+      </c>
+      <c r="B3" t="n">
+        <v>-8.743978145912101e-19</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.00012</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-0.06</v>
+      </c>
+      <c r="F3" t="n">
+        <v>-4.371989072956051e-16</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>8.743978145912101e-19</v>
+      </c>
+      <c r="I3" t="n">
+        <v>-0.00012</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>-0.06</v>
+      </c>
+      <c r="L3" t="n">
+        <v>-4.371989072956051e-16</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>0</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.16154</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>-0.16154</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>0</v>
+      </c>
+      <c r="B5" t="n">
+        <v>4.371989072956051e-16</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-0.06</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>40</v>
+      </c>
+      <c r="F5" t="n">
+        <v>2.914659381970701e-13</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>-4.371989072956051e-16</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>20</v>
+      </c>
+      <c r="L5" t="n">
+        <v>1.45732969098535e-13</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>0</v>
+      </c>
+      <c r="B6" t="n">
+        <v>7.2</v>
+      </c>
+      <c r="C6" t="n">
+        <v>-4.371989072956051e-16</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>2.914659381970701e-13</v>
+      </c>
+      <c r="F6" t="n">
+        <v>4800</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>-7.2</v>
+      </c>
+      <c r="I6" t="n">
+        <v>4.371989072956051e-16</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>1.45732969098535e-13</v>
+      </c>
+      <c r="L6" t="n">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>-0.01</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>0</v>
+      </c>
+      <c r="B8" t="n">
+        <v>-0.0144</v>
+      </c>
+      <c r="C8" t="n">
+        <v>8.743978145912101e-19</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>-4.371989072956051e-16</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-7.2</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.0144</v>
+      </c>
+      <c r="I8" t="n">
+        <v>-8.743978145912101e-19</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>-4.371989072956051e-16</v>
+      </c>
+      <c r="L8" t="n">
+        <v>-7.2</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>0</v>
+      </c>
+      <c r="B9" t="n">
+        <v>8.743978145912101e-19</v>
+      </c>
+      <c r="C9" t="n">
+        <v>-0.00012</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="F9" t="n">
+        <v>4.371989072956051e-16</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>-8.743978145912101e-19</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.00012</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="L9" t="n">
+        <v>4.371989072956051e-16</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>0</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>-0.16154</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.16154</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>0</v>
+      </c>
+      <c r="B11" t="n">
+        <v>4.371989072956051e-16</v>
+      </c>
+      <c r="C11" t="n">
+        <v>-0.06</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>20</v>
+      </c>
+      <c r="F11" t="n">
+        <v>1.45732969098535e-13</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>-4.371989072956051e-16</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>40</v>
+      </c>
+      <c r="L11" t="n">
+        <v>2.914659381970701e-13</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>0</v>
+      </c>
+      <c r="B12" t="n">
+        <v>7.2</v>
+      </c>
+      <c r="C12" t="n">
+        <v>-4.371989072956051e-16</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="n">
+        <v>1.45732969098535e-13</v>
+      </c>
+      <c r="F12" t="n">
+        <v>2400</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>-7.2</v>
+      </c>
+      <c r="I12" t="n">
+        <v>4.371989072956051e-16</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>2.914659381970701e-13</v>
+      </c>
+      <c r="L12" t="n">
+        <v>4800</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="n">
+        <v>0.009599999999999999</v>
+      </c>
+      <c r="B1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F1" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="G1" t="n">
+        <v>-0.009599999999999999</v>
+      </c>
+      <c r="H1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L1" t="n">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>-0.02</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>0</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.01152</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-2.88</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>-0.01152</v>
+      </c>
+      <c r="J3" t="n">
+        <v>-2.88</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>0</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>-2.88</v>
+      </c>
+      <c r="D4" t="n">
+        <v>960</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>2.88</v>
+      </c>
+      <c r="J4" t="n">
+        <v>480</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>0</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.32308</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>-0.32308</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>800</v>
+      </c>
+      <c r="G6" t="n">
+        <v>-2.4</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>-0.009599999999999999</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-2.4</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.009599999999999999</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>-2.4</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>0</v>
+      </c>
+      <c r="B8" t="n">
+        <v>-0.02</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>0</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>-0.01152</v>
+      </c>
+      <c r="D9" t="n">
+        <v>2.88</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.01152</v>
+      </c>
+      <c r="J9" t="n">
+        <v>2.88</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>0</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>-2.88</v>
+      </c>
+      <c r="D10" t="n">
+        <v>480</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>2.88</v>
+      </c>
+      <c r="J10" t="n">
+        <v>960</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>0</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-0.32308</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.32308</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>400</v>
+      </c>
+      <c r="G12" t="n">
+        <v>-2.4</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>800</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1378,7 +3415,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>9.6</v>
+        <v>0.00096</v>
       </c>
       <c r="B1" t="n">
         <v>0</v>
@@ -1393,10 +3430,10 @@
         <v>0</v>
       </c>
       <c r="F1" t="n">
-        <v>-24</v>
+        <v>-0.24</v>
       </c>
       <c r="G1" t="n">
-        <v>-9.6</v>
+        <v>-0.00096</v>
       </c>
       <c r="H1" t="n">
         <v>0</v>
@@ -1411,7 +3448,7 @@
         <v>0</v>
       </c>
       <c r="L1" t="n">
-        <v>-24</v>
+        <v>-0.24</v>
       </c>
       <c r="M1" t="n">
         <v>0</v>
@@ -1455,7 +3492,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>0.02</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -1473,7 +3510,7 @@
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>-2</v>
+        <v>-0.02</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -1532,10 +3569,10 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>9.6</v>
+        <v>0.1152</v>
       </c>
       <c r="D3" t="n">
-        <v>24</v>
+        <v>28.8</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
@@ -1550,10 +3587,10 @@
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>-9.6</v>
+        <v>-0.1152</v>
       </c>
       <c r="J3" t="n">
-        <v>24</v>
+        <v>28.8</v>
       </c>
       <c r="K3" t="n">
         <v>0</v>
@@ -1606,10 +3643,10 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>24</v>
+        <v>28.8</v>
       </c>
       <c r="D4" t="n">
-        <v>80</v>
+        <v>9600</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -1624,10 +3661,10 @@
         <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>-24</v>
+        <v>-28.8</v>
       </c>
       <c r="J4" t="n">
-        <v>40</v>
+        <v>4800</v>
       </c>
       <c r="K4" t="n">
         <v>0</v>
@@ -1686,7 +3723,7 @@
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>32.308</v>
+        <v>0.32308</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
@@ -1704,7 +3741,7 @@
         <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>-32.308</v>
+        <v>-0.32308</v>
       </c>
       <c r="L5" t="n">
         <v>0</v>
@@ -1748,7 +3785,7 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-24</v>
+        <v>-0.24</v>
       </c>
       <c r="B6" t="n">
         <v>0</v>
@@ -1766,7 +3803,7 @@
         <v>80</v>
       </c>
       <c r="G6" t="n">
-        <v>24</v>
+        <v>0.24</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
@@ -1822,7 +3859,7 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>-9.6</v>
+        <v>-0.00096</v>
       </c>
       <c r="B7" t="n">
         <v>0</v>
@@ -1837,10 +3874,10 @@
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>24</v>
+        <v>0.24</v>
       </c>
       <c r="G7" t="n">
-        <v>10.6</v>
+        <v>0.01096</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -1855,10 +3892,10 @@
         <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>24</v>
+        <v>0.24</v>
       </c>
       <c r="M7" t="n">
-        <v>-1</v>
+        <v>-0.01</v>
       </c>
       <c r="N7" t="n">
         <v>0</v>
@@ -1899,7 +3936,7 @@
         <v>0</v>
       </c>
       <c r="B8" t="n">
-        <v>-2</v>
+        <v>-0.02</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
@@ -1917,37 +3954,37 @@
         <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>3.2</v>
+        <v>0.0344</v>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>-8.743978145912101e-19</v>
       </c>
       <c r="J8" t="n">
         <v>0</v>
       </c>
       <c r="K8" t="n">
-        <v>0</v>
+        <v>4.371989072956051e-16</v>
       </c>
       <c r="L8" t="n">
-        <v>6</v>
+        <v>7.2</v>
       </c>
       <c r="M8" t="n">
         <v>0</v>
       </c>
       <c r="N8" t="n">
-        <v>-1.2</v>
+        <v>-0.0144</v>
       </c>
       <c r="O8" t="n">
-        <v>0</v>
+        <v>8.743978145912101e-19</v>
       </c>
       <c r="P8" t="n">
         <v>0</v>
       </c>
       <c r="Q8" t="n">
-        <v>0</v>
+        <v>4.371989072956051e-16</v>
       </c>
       <c r="R8" t="n">
-        <v>6</v>
+        <v>7.2</v>
       </c>
       <c r="S8" t="n">
         <v>0</v>
@@ -1976,10 +4013,10 @@
         <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>-9.6</v>
+        <v>-0.1152</v>
       </c>
       <c r="D9" t="n">
-        <v>-24</v>
+        <v>-28.8</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
@@ -1991,37 +4028,37 @@
         <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>-8.743978145912101e-19</v>
       </c>
       <c r="I9" t="n">
-        <v>10.8</v>
+        <v>0.11532</v>
       </c>
       <c r="J9" t="n">
-        <v>-24</v>
+        <v>-28.8</v>
       </c>
       <c r="K9" t="n">
-        <v>-6</v>
+        <v>-0.06</v>
       </c>
       <c r="L9" t="n">
-        <v>0</v>
+        <v>-4.371989072956051e-16</v>
       </c>
       <c r="M9" t="n">
         <v>0</v>
       </c>
       <c r="N9" t="n">
-        <v>0</v>
+        <v>8.743978145912101e-19</v>
       </c>
       <c r="O9" t="n">
-        <v>-1.2</v>
+        <v>-0.00012</v>
       </c>
       <c r="P9" t="n">
         <v>0</v>
       </c>
       <c r="Q9" t="n">
-        <v>-6</v>
+        <v>-0.06</v>
       </c>
       <c r="R9" t="n">
-        <v>0</v>
+        <v>-4.371989072956051e-16</v>
       </c>
       <c r="S9" t="n">
         <v>0</v>
@@ -2050,10 +4087,10 @@
         <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>24</v>
+        <v>28.8</v>
       </c>
       <c r="D10" t="n">
-        <v>40</v>
+        <v>4800</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
@@ -2068,10 +4105,10 @@
         <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>-24</v>
+        <v>-28.8</v>
       </c>
       <c r="J10" t="n">
-        <v>96.154</v>
+        <v>9600.161539999999</v>
       </c>
       <c r="K10" t="n">
         <v>0</v>
@@ -2089,7 +4126,7 @@
         <v>0</v>
       </c>
       <c r="P10" t="n">
-        <v>-16.154</v>
+        <v>-0.16154</v>
       </c>
       <c r="Q10" t="n">
         <v>0</v>
@@ -2130,7 +4167,7 @@
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>-32.308</v>
+        <v>-0.32308</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
@@ -2139,28 +4176,28 @@
         <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>0</v>
+        <v>4.371989072956051e-16</v>
       </c>
       <c r="I11" t="n">
-        <v>-6</v>
+        <v>-0.06</v>
       </c>
       <c r="J11" t="n">
         <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>72.30799999999999</v>
+        <v>40.32308</v>
       </c>
       <c r="L11" t="n">
-        <v>0</v>
+        <v>2.914659381970701e-13</v>
       </c>
       <c r="M11" t="n">
         <v>0</v>
       </c>
       <c r="N11" t="n">
-        <v>0</v>
+        <v>-4.371989072956051e-16</v>
       </c>
       <c r="O11" t="n">
-        <v>6</v>
+        <v>0.06</v>
       </c>
       <c r="P11" t="n">
         <v>0</v>
@@ -2169,7 +4206,7 @@
         <v>20</v>
       </c>
       <c r="R11" t="n">
-        <v>0</v>
+        <v>1.45732969098535e-13</v>
       </c>
       <c r="S11" t="n">
         <v>0</v>
@@ -2192,7 +4229,7 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>-24</v>
+        <v>-0.24</v>
       </c>
       <c r="B12" t="n">
         <v>0</v>
@@ -2210,40 +4247,40 @@
         <v>40</v>
       </c>
       <c r="G12" t="n">
-        <v>24</v>
+        <v>0.24</v>
       </c>
       <c r="H12" t="n">
-        <v>6</v>
+        <v>7.2</v>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>-4.371989072956051e-16</v>
       </c>
       <c r="J12" t="n">
         <v>0</v>
       </c>
       <c r="K12" t="n">
-        <v>0</v>
+        <v>2.914659381970701e-13</v>
       </c>
       <c r="L12" t="n">
-        <v>120</v>
+        <v>4880</v>
       </c>
       <c r="M12" t="n">
         <v>0</v>
       </c>
       <c r="N12" t="n">
-        <v>-6</v>
+        <v>-7.2</v>
       </c>
       <c r="O12" t="n">
-        <v>0</v>
+        <v>4.371989072956051e-16</v>
       </c>
       <c r="P12" t="n">
         <v>0</v>
       </c>
       <c r="Q12" t="n">
-        <v>0</v>
+        <v>1.45732969098535e-13</v>
       </c>
       <c r="R12" t="n">
-        <v>20</v>
+        <v>2400</v>
       </c>
       <c r="S12" t="n">
         <v>0</v>
@@ -2284,7 +4321,7 @@
         <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>-1</v>
+        <v>-0.01</v>
       </c>
       <c r="H13" t="n">
         <v>0</v>
@@ -2302,7 +4339,7 @@
         <v>0</v>
       </c>
       <c r="M13" t="n">
-        <v>10.6</v>
+        <v>0.0196</v>
       </c>
       <c r="N13" t="n">
         <v>0</v>
@@ -2317,10 +4354,10 @@
         <v>0</v>
       </c>
       <c r="R13" t="n">
-        <v>24</v>
+        <v>2.4</v>
       </c>
       <c r="S13" t="n">
-        <v>-9.6</v>
+        <v>-0.009599999999999999</v>
       </c>
       <c r="T13" t="n">
         <v>0</v>
@@ -2335,7 +4372,7 @@
         <v>0</v>
       </c>
       <c r="X13" t="n">
-        <v>24</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="14">
@@ -2361,43 +4398,43 @@
         <v>0</v>
       </c>
       <c r="H14" t="n">
-        <v>-1.2</v>
+        <v>-0.0144</v>
       </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>8.743978145912101e-19</v>
       </c>
       <c r="J14" t="n">
         <v>0</v>
       </c>
       <c r="K14" t="n">
-        <v>0</v>
+        <v>-4.371989072956051e-16</v>
       </c>
       <c r="L14" t="n">
-        <v>-6</v>
+        <v>-7.2</v>
       </c>
       <c r="M14" t="n">
         <v>0</v>
       </c>
       <c r="N14" t="n">
-        <v>3.2</v>
+        <v>0.0344</v>
       </c>
       <c r="O14" t="n">
-        <v>0</v>
+        <v>-8.743978145912101e-19</v>
       </c>
       <c r="P14" t="n">
         <v>0</v>
       </c>
       <c r="Q14" t="n">
-        <v>0</v>
+        <v>-4.371989072956051e-16</v>
       </c>
       <c r="R14" t="n">
-        <v>-6</v>
+        <v>-7.2</v>
       </c>
       <c r="S14" t="n">
         <v>0</v>
       </c>
       <c r="T14" t="n">
-        <v>-2</v>
+        <v>-0.02</v>
       </c>
       <c r="U14" t="n">
         <v>0</v>
@@ -2435,37 +4472,37 @@
         <v>0</v>
       </c>
       <c r="H15" t="n">
-        <v>0</v>
+        <v>8.743978145912101e-19</v>
       </c>
       <c r="I15" t="n">
-        <v>-1.2</v>
+        <v>-0.00012</v>
       </c>
       <c r="J15" t="n">
         <v>0</v>
       </c>
       <c r="K15" t="n">
-        <v>6</v>
+        <v>0.06</v>
       </c>
       <c r="L15" t="n">
-        <v>0</v>
+        <v>4.371989072956051e-16</v>
       </c>
       <c r="M15" t="n">
         <v>0</v>
       </c>
       <c r="N15" t="n">
-        <v>0</v>
+        <v>-8.743978145912101e-19</v>
       </c>
       <c r="O15" t="n">
-        <v>10.8</v>
+        <v>0.01164</v>
       </c>
       <c r="P15" t="n">
-        <v>-24</v>
+        <v>-2.88</v>
       </c>
       <c r="Q15" t="n">
-        <v>6</v>
+        <v>0.06</v>
       </c>
       <c r="R15" t="n">
-        <v>0</v>
+        <v>4.371989072956051e-16</v>
       </c>
       <c r="S15" t="n">
         <v>0</v>
@@ -2474,10 +4511,10 @@
         <v>0</v>
       </c>
       <c r="U15" t="n">
-        <v>-9.6</v>
+        <v>-0.01152</v>
       </c>
       <c r="V15" t="n">
-        <v>-24</v>
+        <v>-2.88</v>
       </c>
       <c r="W15" t="n">
         <v>0</v>
@@ -2515,7 +4552,7 @@
         <v>0</v>
       </c>
       <c r="J16" t="n">
-        <v>-16.154</v>
+        <v>-0.16154</v>
       </c>
       <c r="K16" t="n">
         <v>0</v>
@@ -2530,10 +4567,10 @@
         <v>0</v>
       </c>
       <c r="O16" t="n">
-        <v>-24</v>
+        <v>-2.88</v>
       </c>
       <c r="P16" t="n">
-        <v>96.154</v>
+        <v>960.1615399999999</v>
       </c>
       <c r="Q16" t="n">
         <v>0</v>
@@ -2548,10 +4585,10 @@
         <v>0</v>
       </c>
       <c r="U16" t="n">
-        <v>24</v>
+        <v>2.88</v>
       </c>
       <c r="V16" t="n">
-        <v>40</v>
+        <v>480</v>
       </c>
       <c r="W16" t="n">
         <v>0</v>
@@ -2583,10 +4620,10 @@
         <v>0</v>
       </c>
       <c r="H17" t="n">
-        <v>0</v>
+        <v>4.371989072956051e-16</v>
       </c>
       <c r="I17" t="n">
-        <v>-6</v>
+        <v>-0.06</v>
       </c>
       <c r="J17" t="n">
         <v>0</v>
@@ -2595,25 +4632,25 @@
         <v>20</v>
       </c>
       <c r="L17" t="n">
-        <v>0</v>
+        <v>1.45732969098535e-13</v>
       </c>
       <c r="M17" t="n">
         <v>0</v>
       </c>
       <c r="N17" t="n">
-        <v>0</v>
+        <v>-4.371989072956051e-16</v>
       </c>
       <c r="O17" t="n">
-        <v>6</v>
+        <v>0.06</v>
       </c>
       <c r="P17" t="n">
         <v>0</v>
       </c>
       <c r="Q17" t="n">
-        <v>72.30799999999999</v>
+        <v>40.32308</v>
       </c>
       <c r="R17" t="n">
-        <v>0</v>
+        <v>2.914659381970701e-13</v>
       </c>
       <c r="S17" t="n">
         <v>0</v>
@@ -2628,7 +4665,7 @@
         <v>0</v>
       </c>
       <c r="W17" t="n">
-        <v>-32.308</v>
+        <v>-0.32308</v>
       </c>
       <c r="X17" t="n">
         <v>0</v>
@@ -2657,40 +4694,40 @@
         <v>0</v>
       </c>
       <c r="H18" t="n">
-        <v>6</v>
+        <v>7.2</v>
       </c>
       <c r="I18" t="n">
-        <v>0</v>
+        <v>-4.371989072956051e-16</v>
       </c>
       <c r="J18" t="n">
         <v>0</v>
       </c>
       <c r="K18" t="n">
-        <v>0</v>
+        <v>1.45732969098535e-13</v>
       </c>
       <c r="L18" t="n">
-        <v>20</v>
+        <v>2400</v>
       </c>
       <c r="M18" t="n">
-        <v>24</v>
+        <v>2.4</v>
       </c>
       <c r="N18" t="n">
-        <v>-6</v>
+        <v>-7.2</v>
       </c>
       <c r="O18" t="n">
-        <v>0</v>
+        <v>4.371989072956051e-16</v>
       </c>
       <c r="P18" t="n">
         <v>0</v>
       </c>
       <c r="Q18" t="n">
-        <v>0</v>
+        <v>2.914659381970701e-13</v>
       </c>
       <c r="R18" t="n">
-        <v>120</v>
+        <v>5600</v>
       </c>
       <c r="S18" t="n">
-        <v>-24</v>
+        <v>-2.4</v>
       </c>
       <c r="T18" t="n">
         <v>0</v>
@@ -2705,7 +4742,7 @@
         <v>0</v>
       </c>
       <c r="X18" t="n">
-        <v>40</v>
+        <v>400</v>
       </c>
     </row>
     <row r="19">
@@ -2746,7 +4783,7 @@
         <v>0</v>
       </c>
       <c r="M19" t="n">
-        <v>-9.6</v>
+        <v>-0.009599999999999999</v>
       </c>
       <c r="N19" t="n">
         <v>0</v>
@@ -2761,10 +4798,10 @@
         <v>0</v>
       </c>
       <c r="R19" t="n">
-        <v>-24</v>
+        <v>-2.4</v>
       </c>
       <c r="S19" t="n">
-        <v>9.6</v>
+        <v>0.009599999999999999</v>
       </c>
       <c r="T19" t="n">
         <v>0</v>
@@ -2779,7 +4816,7 @@
         <v>0</v>
       </c>
       <c r="X19" t="n">
-        <v>-24</v>
+        <v>-2.4</v>
       </c>
     </row>
     <row r="20">
@@ -2823,7 +4860,7 @@
         <v>0</v>
       </c>
       <c r="N20" t="n">
-        <v>-2</v>
+        <v>-0.02</v>
       </c>
       <c r="O20" t="n">
         <v>0</v>
@@ -2841,7 +4878,7 @@
         <v>0</v>
       </c>
       <c r="T20" t="n">
-        <v>2</v>
+        <v>0.02</v>
       </c>
       <c r="U20" t="n">
         <v>0</v>
@@ -2900,10 +4937,10 @@
         <v>0</v>
       </c>
       <c r="O21" t="n">
-        <v>-9.6</v>
+        <v>-0.01152</v>
       </c>
       <c r="P21" t="n">
-        <v>24</v>
+        <v>2.88</v>
       </c>
       <c r="Q21" t="n">
         <v>0</v>
@@ -2918,10 +4955,10 @@
         <v>0</v>
       </c>
       <c r="U21" t="n">
-        <v>9.6</v>
+        <v>0.01152</v>
       </c>
       <c r="V21" t="n">
-        <v>24</v>
+        <v>2.88</v>
       </c>
       <c r="W21" t="n">
         <v>0</v>
@@ -2974,10 +5011,10 @@
         <v>0</v>
       </c>
       <c r="O22" t="n">
-        <v>-24</v>
+        <v>-2.88</v>
       </c>
       <c r="P22" t="n">
-        <v>40</v>
+        <v>480</v>
       </c>
       <c r="Q22" t="n">
         <v>0</v>
@@ -2992,10 +5029,10 @@
         <v>0</v>
       </c>
       <c r="U22" t="n">
-        <v>24</v>
+        <v>2.88</v>
       </c>
       <c r="V22" t="n">
-        <v>80</v>
+        <v>960</v>
       </c>
       <c r="W22" t="n">
         <v>0</v>
@@ -3054,7 +5091,7 @@
         <v>0</v>
       </c>
       <c r="Q23" t="n">
-        <v>-32.308</v>
+        <v>-0.32308</v>
       </c>
       <c r="R23" t="n">
         <v>0</v>
@@ -3072,7 +5109,7 @@
         <v>0</v>
       </c>
       <c r="W23" t="n">
-        <v>32.308</v>
+        <v>0.32308</v>
       </c>
       <c r="X23" t="n">
         <v>0</v>
@@ -3116,7 +5153,7 @@
         <v>0</v>
       </c>
       <c r="M24" t="n">
-        <v>24</v>
+        <v>2.4</v>
       </c>
       <c r="N24" t="n">
         <v>0</v>
@@ -3131,10 +5168,10 @@
         <v>0</v>
       </c>
       <c r="R24" t="n">
-        <v>40</v>
+        <v>400</v>
       </c>
       <c r="S24" t="n">
-        <v>-24</v>
+        <v>-2.4</v>
       </c>
       <c r="T24" t="n">
         <v>0</v>
@@ -3149,7 +5186,7 @@
         <v>0</v>
       </c>
       <c r="X24" t="n">
-        <v>80</v>
+        <v>800</v>
       </c>
     </row>
   </sheetData>
@@ -3157,7 +5194,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3173,22 +5210,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>1.75973421993209</v>
+        <v>0.175973421993209</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1.999697977195557</v>
+        <v>0.1999697977195557</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1.523852505115035e-16</v>
+        <v>1.523852505115035e-17</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2.077980688793229e-16</v>
+        <v>2.077980688793229e-15</v>
       </c>
     </row>
     <row r="5">
@@ -3198,87 +5235,87 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-2.399637572634668</v>
+        <v>-23.99637572634668</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>-0.2604892769431992</v>
+        <v>-0.02604892769431993</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>-8.517553539055594</v>
+        <v>-0.8517553539055595</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>-4.95898677672336e-16</v>
+        <v>-4.958986776723362e-17</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>-3.116971033189843e-16</v>
+        <v>-3.116971033189843e-15</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>1.340988245066352e-15</v>
+        <v>1.340988245066352e-14</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>-16.70624594608282</v>
+        <v>-67.06245946082819</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>4.019921474070845</v>
+        <v>0.4019921474070846</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>4.516949493446706</v>
+        <v>0.4516949493446706</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>3.315902659243339e-16</v>
+        <v>3.315902659243338e-17</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>-6.926602295977432e-17</v>
+        <v>-6.92660229597743e-16</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>-3.122849337825751e-16</v>
+        <v>-3.122849337825752e-15</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>6.556354712334473</v>
+        <v>65.56354712334472</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>4.479323468918047</v>
+        <v>0.4479323468918047</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>3.999395954391114</v>
+        <v>0.3999395954391113</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>3.878897285747362e-16</v>
+        <v>3.878897285747361e-17</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>2.770640918390973e-16</v>
+        <v>2.770640918390972e-15</v>
       </c>
     </row>
     <row r="23">
@@ -3288,7 +5325,7 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>-3.199516763512891</v>
+        <v>-31.99516763512891</v>
       </c>
     </row>
   </sheetData>
@@ -3296,7 +5333,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3342,62 +5379,62 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>-0.1157526144211102</v>
+        <v>17.37620386288346</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>-2.942887987078604</v>
+        <v>-37.21942751395427</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>-1.282284252159821e-16</v>
+        <v>-1.691847880748255e-15</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>-3.587155844659385e-17</v>
+        <v>-5.399783743506291e-18</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>1.225105798676267e-17</v>
+        <v>5.987737404744856e-16</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>0.02615356585723976</v>
+        <v>0.03838797970722242</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>-0.3388028553468134</v>
+        <v>22.57052371612574</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>0.9425859642741589</v>
+        <v>17.21640728590984</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>1.214619620280307e-17</v>
+        <v>7.244959723050406e-15</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>-3.71514933584435e-18</v>
+        <v>2.10089142830294e-17</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>-1.935544921765973e-17</v>
+        <v>-3.379423834713422e-16</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>0.3123116302635815</v>
+        <v>0.05557163383327336</v>
       </c>
     </row>
     <row r="19">
@@ -3428,139 +5465,6 @@
     <row r="24">
       <c r="A24" t="n">
         <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:L3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="n">
-        <v>-1.276194702063186</v>
-      </c>
-      <c r="B1" t="n">
-        <v>3.886077996961652</v>
-      </c>
-      <c r="C1" t="n">
-        <v>2.176902288436723e-16</v>
-      </c>
-      <c r="D1" t="n">
-        <v>1.434821798440494e-15</v>
-      </c>
-      <c r="E1" t="n">
-        <v>-3.958071814363284e-16</v>
-      </c>
-      <c r="F1" t="n">
-        <v>0.6677174608176137</v>
-      </c>
-      <c r="G1" t="n">
-        <v>-3.723050240925706</v>
-      </c>
-      <c r="H1" t="n">
-        <v>-8.885322939950544</v>
-      </c>
-      <c r="I1" t="n">
-        <v>-6.506028723422618e-16</v>
-      </c>
-      <c r="J1" t="n">
-        <v>5.194546327750471e-16</v>
-      </c>
-      <c r="K1" t="n">
-        <v>3.958071814363284e-16</v>
-      </c>
-      <c r="L1" t="n">
-        <v>-4.285233836479466</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>3.723050240925704</v>
-      </c>
-      <c r="B2" t="n">
-        <v>8.885322939950541</v>
-      </c>
-      <c r="C2" t="n">
-        <v>6.506028723422621e-16</v>
-      </c>
-      <c r="D2" t="n">
-        <v>-5.194546327750473e-16</v>
-      </c>
-      <c r="E2" t="n">
-        <v>-3.958071814363287e-16</v>
-      </c>
-      <c r="F2" t="n">
-        <v>4.285233836479467</v>
-      </c>
-      <c r="G2" t="n">
-        <v>-3.723050240925704</v>
-      </c>
-      <c r="H2" t="n">
-        <v>-0.8853229399505396</v>
-      </c>
-      <c r="I2" t="n">
-        <v>-1.607441526833208e-16</v>
-      </c>
-      <c r="J2" t="n">
-        <v>5.194546327750473e-16</v>
-      </c>
-      <c r="K2" t="n">
-        <v>6.253358533241503e-16</v>
-      </c>
-      <c r="L2" t="n">
-        <v>-16.05378270188478</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>3.723050240925701</v>
-      </c>
-      <c r="B3" t="n">
-        <v>0.8853229399505393</v>
-      </c>
-      <c r="C3" t="n">
-        <v>1.607441526833206e-16</v>
-      </c>
-      <c r="D3" t="n">
-        <v>-5.194546327750473e-16</v>
-      </c>
-      <c r="E3" t="n">
-        <v>-6.253358533241507e-16</v>
-      </c>
-      <c r="F3" t="n">
-        <v>16.05378270188478</v>
-      </c>
-      <c r="G3" t="n">
-        <v>-8.722295183914593</v>
-      </c>
-      <c r="H3" t="n">
-        <v>-5.884567882939431</v>
-      </c>
-      <c r="I3" t="n">
-        <v>-5.936567961819101e-16</v>
-      </c>
-      <c r="J3" t="n">
-        <v>-7.171787741401449e-16</v>
-      </c>
-      <c r="K3" t="n">
-        <v>6.253358533241507e-16</v>
-      </c>
-      <c r="L3" t="n">
-        <v>7.560713445732629</v>
       </c>
     </row>
   </sheetData>

</xml_diff>